<commit_message>
Arreglado Versión Excel No Español, Categorías y arreglos varios
</commit_message>
<xml_diff>
--- a/0.EJEMPLOS_EXAMPLES/FastTest PlugIn - DataBase_Examples - English.xlsx
+++ b/0.EJEMPLOS_EXAMPLES/FastTest PlugIn - DataBase_Examples - English.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milag\Desktop\FastTest_PlugIn_V78\0.EJEMPLOS_EXAMPLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milag\Desktop\FTP_81\0.EJEMPLOS_EXAMPLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1120CD-2905-4E1F-9434-57C575AA61C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44935B7-5ADB-466E-9F99-F9D48E8DE430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12266" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="6" r:id="rId1"/>
@@ -630,7 +630,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="976">
   <si>
     <t>MILAGROS HUERTA GÓMEZ DE MERODIO</t>
   </si>
@@ -3619,6 +3619,20 @@
 3. Mark the Colors: &lt;br/&gt;{1:MCHS:=White#Very good~=Chair#Very good~%-50%Table~%-50%Floor}&lt;br/&gt; 
 4. Mark the Colors: &lt;br/&gt;{1:MRHS:=White#Very good~=Black#Very good~%-50%Table~%-50%Chair}&lt;br/&gt;
 5. Mark the Colors: &lt;br/&gt;{1:MRS:=White#Very good~=Orange#Correct~=Blue~%-50%Table~%-50%Chair#Not a color~%-50%Pen}</t>
+  </si>
+  <si>
+    <t>Images and Formulas</t>
+  </si>
+  <si>
+    <t>Select the correct formula: [[[{1:MCVS:~%100%\(\frac{\cos^2(x)\}{x-1\}\)#OK~%0%\(-\frac{\cos^2(x)\}{x-1\}\)#~%0%\(\frac{\cos(x)\}{x-1\}-\frac{\sin(x)\}{(x-1)^2\}\)#}]]]&lt;br&gt;
+Select the correct Image: [[[{1:MCVS:~%100%&lt;img src = "https://dl.dropboxusercontent.com/s/oh1ssro2fay57yo/Alumno_hablando_rapido.gif" width = "" height = "100"&gt;#OK~%0%&lt;img src = "https://dl.dropboxusercontent.com/s/2smr0aec6oujybp/Antonio_hablando_izq_rapido.gif" width = "" height = "120"&gt;#NO~%0%&lt;img src = "https://dl.dropboxusercontent.com/s/qfxkf5guj4pjibp/Profe_hablando_rapido.gif" width = "" height = "100"&gt;#NO}]]]</t>
+  </si>
+  <si>
+    <t>Formulas</t>
+  </si>
+  <si>
+    <t>Select the correct formula: &lt;br&gt;
+{1:MCHS:~%100%\(\frac{\cos^2(x)\}{x-1\}\)#~%0%\(-\frac{\cos^2(x)\}{x-1\}\)#}&lt;br&gt;</t>
   </si>
 </sst>
 </file>
@@ -5350,10 +5364,54 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="348">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6392,36 +6450,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -8205,20 +8233,6 @@
         <patternFill>
           <fgColor indexed="64"/>
           <bgColor rgb="FF005877"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -15613,10 +15627,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="4" name="MENU">
+        <xdr:cNvPr id="2" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{652995F8-911C-4DCC-BFDE-18A844C10A6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C708AEC-2EF6-49D5-ABAE-AFF8A0E8948D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15632,10 +15646,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="FONDO BLANCO">
+          <xdr:cNvPr id="3" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A32D1AD-9634-82DC-FF76-AA1B4B313291}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA223F18-D779-AA73-7EB6-5EE0D7DA1166}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -15683,10 +15697,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="6" name="FTP-MOODLE">
+          <xdr:cNvPr id="15" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB0E3F40-7831-3FB0-0962-7A0B778E1859}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E72D145-13E7-8CB6-C8DA-64149D40BF08}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -15702,10 +15716,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="35" name="Moodle">
+            <xdr:cNvPr id="27" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9ABC2B0-DD3E-99FC-804B-5A0FA36D7174}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF6DC1EF-E7F9-EFCE-829B-8E1F14C26D8D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15730,10 +15744,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="36" name="FTP">
+            <xdr:cNvPr id="28" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA470E1-F4DA-6732-5977-DAA06FD9B490}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4017BF2B-2DD2-163C-AD72-2C081F7097C3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15759,11 +15773,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="DICCIONARIO">
+          <xdr:cNvPr id="16" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EBE43D0-E0A7-20C6-4702-7582F6BE30E5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10C92BD7-DB40-0380-945B-39426A40739A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -15811,11 +15825,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="INICIO">
+          <xdr:cNvPr id="17" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884A7CC4-D0E1-C088-2C04-231F1D1C5C00}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A857109-0B9E-2191-564A-3C962CD832BA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -15863,10 +15877,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="9" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="18" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02C4FF12-B8A4-2A40-3FC6-BEB4A31858F8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642AC39B-C5D6-171A-0043-ADBCB9B019BA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -15882,11 +15896,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="OM">
+            <xdr:cNvPr id="19" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4217BED3-68A8-2ABB-EE41-A83B095AAD43}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EEE3E61-73B5-6BC4-2438-7099EF2AE984}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15934,11 +15948,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="O2">
+            <xdr:cNvPr id="20" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E42BD4F2-3855-064F-0954-3CF2DCC87ED0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD22B59-9E3C-B366-5E0C-F94B239C3FFF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -15986,11 +16000,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="VF">
+            <xdr:cNvPr id="21" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F614AB0F-234F-A105-A21E-2C75DAE5876C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85615DE5-EB16-75BE-B929-B0B2FA515EBC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16038,11 +16052,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="EM">
+            <xdr:cNvPr id="22" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D484B2B-423F-C633-0AFE-9C6DF00CEAEB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0784F9D5-40BE-E2E9-9B34-A7E1B7F78B31}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16090,11 +16104,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="RC">
+            <xdr:cNvPr id="23" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37D1C7E4-4B2E-3849-C0AE-DA4D841819B7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9133426-A9F1-FDBB-D5BC-7A7BAC0C676C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16142,11 +16156,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="PP">
+            <xdr:cNvPr id="24" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DABB53B-BECF-8A54-D861-081F84BA86DB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{643E8319-349F-B85E-9419-EE2D21613DCB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16194,11 +16208,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="33" name="EN">
+            <xdr:cNvPr id="25" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB048C99-ECFF-9749-9A31-D642DB02056F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07A8E328-6C17-E157-C926-7499AFCFEC2F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16246,11 +16260,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="34" name="CL">
+            <xdr:cNvPr id="26" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32B36D06-E460-58EA-75A6-54A0E80212B0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADE066D-01A7-4BB7-F3FA-C312665FF06F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16376,10 +16390,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="MENU">
+        <xdr:cNvPr id="16" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEC6EDE5-1AE1-4BFC-AF12-893B1A34C1BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{196B32A8-B4B3-4DFD-B9F7-01F28198F247}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16395,10 +16409,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="FONDO BLANCO">
+          <xdr:cNvPr id="17" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CACEB20F-85C7-90BF-FFA6-15237A144878}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1571571E-FBB0-43EE-2A90-84903B11ED9E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -16446,10 +16460,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="FTP-MOODLE">
+          <xdr:cNvPr id="18" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AD0685C-B8B3-CB79-A47D-08187FCD8CBF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82A6BA1B-A130-C97F-D53A-0C4E4E995544}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -16465,10 +16479,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Moodle">
+            <xdr:cNvPr id="30" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{680EF89F-D3E8-CAE3-C3E4-858777B2D501}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{302F1EB7-ECA8-5A0C-058D-7787FCECEA1A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16493,10 +16507,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="34" name="FTP">
+            <xdr:cNvPr id="31" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FABF1D3-50E5-EB7E-828B-9EBCDB4166E9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A09CFB45-2D71-4150-7A6A-C568F3A4112C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16522,11 +16536,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="DICCIONARIO">
+          <xdr:cNvPr id="19" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E504AC-B225-90B7-783F-CA1F9E8FC41D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{048A8CB7-AB59-22AC-5FC2-B633940A3F84}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -16574,11 +16588,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="INICIO">
+          <xdr:cNvPr id="20" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B41A40CF-7BAD-6587-6311-8109D8B50169}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F014122-8DB7-B7D4-AE0A-F596B295653C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -16626,10 +16640,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="21" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86EF39A9-71F3-A363-E964-B90F9DD94C5D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA079406-5CE9-EF74-028D-4B1C8D39297F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -16645,11 +16659,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="OM">
+            <xdr:cNvPr id="22" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{762E515B-D66F-D8BF-34C9-B6296FA2CF79}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19724EE2-2D95-D1C9-6B22-1D8793759A52}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16697,11 +16711,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="O2">
+            <xdr:cNvPr id="23" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5175CF93-9BA7-A465-1A3C-67752FF351A9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5BCB8BA-EDAB-804E-E27C-E6E9D89E8AC9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16749,11 +16763,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="VF">
+            <xdr:cNvPr id="24" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED8271A-75C4-5363-47FD-D600D1BC1C42}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2270863D-4BEB-277D-FECC-921549315015}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16801,11 +16815,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="EM">
+            <xdr:cNvPr id="25" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D11C25C-2F5B-67BA-6088-E2E42D4444EC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F0CD89D-EF3A-C29E-9AFE-A464FAB21ED3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16853,11 +16867,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="RC">
+            <xdr:cNvPr id="26" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1830FCC3-F127-09D1-0C63-BB901FEB015C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E48136-161F-88E0-06C4-D635D74FE1D7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16905,11 +16919,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="PP">
+            <xdr:cNvPr id="27" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA77B59A-9CCB-3975-7671-99359D87208D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B89DE7D7-78D1-2D1D-9CCC-4778CCD8CFEC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -16957,11 +16971,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="EN">
+            <xdr:cNvPr id="28" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39399C2A-5F5C-3E76-BF02-A11031A6B921}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7BAC64B-1682-36CA-3D60-C19283EFAFB2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17009,11 +17023,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="CL">
+            <xdr:cNvPr id="29" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D54A7F7-FAFC-CDD8-5B94-FC0FB8392B3E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06047B66-1D57-5B5D-085D-9C6254A0CFCD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17139,10 +17153,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="MENU">
+        <xdr:cNvPr id="16" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B466AD0-B8DA-49D9-96E8-996B4B68FA97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36E22B5A-B60F-4DD4-BA37-426149675AA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17158,10 +17172,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="FONDO BLANCO">
+          <xdr:cNvPr id="17" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9236AD3D-B1EC-C12A-4313-759D96154083}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71187D1F-24EE-02BD-2BA9-53D48C8A4E37}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17209,10 +17223,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="FTP-MOODLE">
+          <xdr:cNvPr id="18" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70C09BF4-716C-D5FA-73A3-39E50639FA99}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9710BF1A-63D2-2CDE-6CC0-BBB162FF9793}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17228,10 +17242,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Moodle">
+            <xdr:cNvPr id="30" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBD1F20D-6991-DAC0-0C0D-FEFF7AFA7CB9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F42221B-71AF-9750-6168-516C1BAB6719}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17256,10 +17270,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="34" name="FTP">
+            <xdr:cNvPr id="31" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33378B1F-D77E-9BC4-13C7-8AA0A5DEB9E2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5F87CA7-F370-B075-784F-E59FA3675ED7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17285,11 +17299,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="DICCIONARIO">
+          <xdr:cNvPr id="19" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F69E77A-A1B1-9944-3270-942402A83987}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B20148A0-15D8-B5EF-C7E1-6A2F0AE436F3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17337,11 +17351,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="INICIO">
+          <xdr:cNvPr id="20" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{506D1C52-BF58-43C8-65AD-3838C1FB9005}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A498867-D6FA-DCE4-DEAE-FA50FD84F37C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17389,10 +17403,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="21" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C53F133A-94EC-D8B2-453B-A5096091EEEA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2499E444-D251-171C-9823-6A14F3BBD753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17408,11 +17422,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="OM">
+            <xdr:cNvPr id="22" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4D27DB3-C1DA-D4CD-890C-D53ACA6D5F64}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F08C1F2F-6C3E-27E9-AC95-C5BD06329886}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17460,11 +17474,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="O2">
+            <xdr:cNvPr id="23" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DC4A44-6B9C-90B1-5B47-6964C9D64A38}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26A3F4D4-A828-695D-F4B9-7903C7F8AA9A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17512,11 +17526,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="VF">
+            <xdr:cNvPr id="24" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37F0CB82-B1A9-4DC7-84D9-372F1D5A02E9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D5030B-B41F-A43E-CFA6-1CF8C951E6A5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17564,11 +17578,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="EM">
+            <xdr:cNvPr id="25" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDBED940-5D18-0EB9-A9AB-002592D3AB44}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{484D413D-02D5-C737-4746-73144365AE73}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17616,11 +17630,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="RC">
+            <xdr:cNvPr id="26" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B54ACBC-3E90-5785-B89C-4EF648BB41DC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96503DEF-24F3-CCD9-C966-70E51EFBEA2F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17668,11 +17682,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="PP">
+            <xdr:cNvPr id="27" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13D72AED-B118-044F-B32F-640559E15BE4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{147D5DE1-6126-C5DD-C218-56587810E23A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17720,11 +17734,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="EN">
+            <xdr:cNvPr id="28" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6B47383-10F7-C479-C6DD-50B8A69230EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8593670D-AB65-C164-D772-75C74EB24CD9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17772,11 +17786,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="CL">
+            <xdr:cNvPr id="29" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C77D6D25-356F-BE8E-6AB7-72E5E5F018DF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12D74C39-0087-AD36-9638-6534B6051303}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -17902,10 +17916,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="MENU">
+        <xdr:cNvPr id="16" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B467CDBA-296D-461B-9C8D-DEA3B2E60460}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1019C18-24B8-4542-9058-947CA6F4D06F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17921,10 +17935,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="FONDO BLANCO">
+          <xdr:cNvPr id="17" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9A62C90-F812-CA8B-AB59-EC6B79B7ED2D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3708BB3-CF88-742B-1D1E-4BC1E9932BF4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17972,10 +17986,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="FTP-MOODLE">
+          <xdr:cNvPr id="18" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9937D2-52DA-1721-0F6B-53F684E0258E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC339E6B-8657-4D0D-3DD5-CF9E58155560}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -17991,10 +18005,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Moodle">
+            <xdr:cNvPr id="30" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D76E5450-87A7-CB43-99B7-CA02896D26C6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55AA1147-D573-E03A-222D-0FC112079612}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18019,10 +18033,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="34" name="FTP">
+            <xdr:cNvPr id="31" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEA64456-11D0-F941-DD02-995183B4CF35}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436D0B59-821E-6C38-77FC-32D666D042C8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18048,11 +18062,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="DICCIONARIO">
+          <xdr:cNvPr id="19" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68AAE4D3-8373-94CE-1522-D8DD6990323C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03F16383-E013-3243-297C-A68393946C99}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18100,11 +18114,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="INICIO">
+          <xdr:cNvPr id="20" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{137D1F40-4AE4-21CE-6374-2E169F0520ED}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E59A2D14-61F7-2C8C-77E1-A3888D07F556}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18152,10 +18166,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="21" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40916050-C023-0059-B00E-7887515C0EAB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F7B6A5F-AD4E-1D8E-B104-BC31878B8BFF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18171,11 +18185,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="OM">
+            <xdr:cNvPr id="22" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{001F485E-D4D4-F8D4-F9E8-ECDA7039621F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54D8E37-66B4-B026-F8F6-F938235FB93A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18223,11 +18237,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="O2">
+            <xdr:cNvPr id="23" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C686B9F-5229-9969-B209-2117828E00D8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F532E687-ACC4-4E3B-D9AA-AA7A75D3D10B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18275,11 +18289,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="VF">
+            <xdr:cNvPr id="24" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5132C1D4-8F88-E865-B713-76B185BB66A8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41ADAD94-1703-AFAA-EDD5-A783880B4910}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18327,11 +18341,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="EM">
+            <xdr:cNvPr id="25" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A871BD4-6D22-0764-9066-20175567E603}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37C83DAC-ABCF-9009-FB85-B62881BB2D90}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18379,11 +18393,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="RC">
+            <xdr:cNvPr id="26" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84EC3B1-D8A0-D513-CF5F-335DE48C43AB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64495317-DFBF-99AE-7A4E-224DB289389A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18431,11 +18445,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="PP">
+            <xdr:cNvPr id="27" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28B379C-0E7E-A902-011E-441214217FA4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443DB84F-0146-4A35-AFE5-6E2E84C710CA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18483,11 +18497,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="EN">
+            <xdr:cNvPr id="28" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3993BBC4-FA36-147C-EFDB-074EE689CBBF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08A04E66-DE2E-F99A-DD8C-D172687E73AC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18535,11 +18549,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="CL">
+            <xdr:cNvPr id="29" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1DCC4D6-833E-C0F2-2A92-83113F0F2B5B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F93EEA83-21DE-D548-3D66-21C141A032C7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18665,10 +18679,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="MENU">
+        <xdr:cNvPr id="16" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17873629-0592-4E2C-8702-D4461B2E8F95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26ABC3B-7975-46AF-AF55-ECCEEF6DDB64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18684,10 +18698,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="FONDO BLANCO">
+          <xdr:cNvPr id="17" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14A685D3-9FB2-346B-5710-3A3C28700665}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65855BFA-742D-0C1E-DD75-0CA1EBEA5DCC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18735,10 +18749,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="FTP-MOODLE">
+          <xdr:cNvPr id="18" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A31E8E54-5C35-4838-263A-A9F73E46DC28}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B2BBA9-9CC7-0E8D-9254-2048E2C4493C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18754,10 +18768,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Moodle">
+            <xdr:cNvPr id="30" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B7AEB97-4ACE-ED2A-3FD0-516DE39B35EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E313A4B-FE54-2858-EDF7-80A31159C245}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18782,10 +18796,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="34" name="FTP">
+            <xdr:cNvPr id="31" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688B47F1-BDCD-503A-D722-0D70F4BDFB52}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9836296-EFFD-0819-3D5D-6542912445D8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18811,11 +18825,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="DICCIONARIO">
+          <xdr:cNvPr id="19" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5414375B-398C-DDCD-157A-A085AF6324EF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{710F608B-B6C4-52AF-93BE-0527590E30CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18863,11 +18877,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="INICIO">
+          <xdr:cNvPr id="20" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DE764EE-B5FD-65C1-6F1A-66CFC751830D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C4FEA0-AF99-EE25-8797-36ACD61D608A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18915,10 +18929,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="21" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0D48155-BE49-0D43-1584-F1954B8DA366}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F23F42C-3646-361D-432E-8B61CD76A45D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -18934,11 +18948,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="OM">
+            <xdr:cNvPr id="22" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63098759-A9D4-EF37-952D-DCA5C319541C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BB3188E-4891-EDAC-5D25-7E22FBF17D9D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -18986,11 +19000,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="O2">
+            <xdr:cNvPr id="23" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE55E101-02E5-438C-C659-DD443D23EFA4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{379677A0-74EE-F535-5C29-046089FF9F07}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19038,11 +19052,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="VF">
+            <xdr:cNvPr id="24" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21DB1878-0107-8463-267E-CE6E2738380E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA5396B-C692-7E6A-FB8E-A9577FC01494}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19090,11 +19104,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="EM">
+            <xdr:cNvPr id="25" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08A95079-8A4A-EC4A-6DBA-D2FE71AF552D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69D639BA-9EC0-90F7-3B9E-BA9C8019A4E8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19142,11 +19156,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="RC">
+            <xdr:cNvPr id="26" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00E80461-B320-AF0D-4FC0-CA002DCE0210}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1D345-793A-ADD3-29BD-7A7F8AA3E7D5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19194,11 +19208,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="PP">
+            <xdr:cNvPr id="27" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{166B77C8-F84C-5E2C-405A-469BD1648515}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18FDB793-ACE3-CBEC-F2C6-9661B928F4A3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19246,11 +19260,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="EN">
+            <xdr:cNvPr id="28" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73936681-3612-6CAB-BC33-2F5FBB0E9308}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE3A20AE-1704-9310-5EE3-EC1E507CD759}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19298,11 +19312,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="CL">
+            <xdr:cNvPr id="29" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B42E28D0-6B13-B229-FF44-609C624BD96C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD29E0B-0811-988A-4BE2-A7A0801EB9BE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19428,10 +19442,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="MENU">
+        <xdr:cNvPr id="16" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3A48975-AA85-47AE-9850-BC25D8E02023}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A29145A-5A79-4C89-A5DC-0511335D7AB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19447,10 +19461,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="FONDO BLANCO">
+          <xdr:cNvPr id="17" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA16C04-C3A0-3AF2-4A06-E73B0FC238C0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BA6790F-631C-9C29-6F0E-C26812F27095}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -19498,10 +19512,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="FTP-MOODLE">
+          <xdr:cNvPr id="18" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAFEECA0-DE2F-B7A0-A330-3CD0224DF19D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E828A7-7F70-3656-4804-F62D26F54695}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -19517,10 +19531,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Moodle">
+            <xdr:cNvPr id="30" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35527B13-D329-C705-140A-8F616254E7AA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0382C5AE-9563-2F64-6CD9-D2917D8248F2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19545,10 +19559,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="34" name="FTP">
+            <xdr:cNvPr id="31" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D088487-AD84-8F03-BAEB-A0B0F6D82EBF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F31888F9-A045-7FB8-7F44-9138ACBC2F63}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19574,11 +19588,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="DICCIONARIO">
+          <xdr:cNvPr id="19" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57049842-A47A-FAA1-F9C4-7570AD81217B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A97A452-1433-0CC7-85C3-201E2C606E5C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -19626,11 +19640,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="INICIO">
+          <xdr:cNvPr id="20" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98D11ED7-4DA2-A159-B512-4F1908FF163F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5162182-0D7E-6546-3C0B-E54F681EFFC7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -19678,10 +19692,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="21" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5116AA22-8335-C167-3A53-B9B9C1E09ADB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91599C1-150A-F0E8-5EC2-49F166009A73}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -19697,11 +19711,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="OM">
+            <xdr:cNvPr id="22" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18D32E6C-8128-D367-C1C7-D5A7DF821D4B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD24B57A-FA08-B46A-6410-707FD6252B13}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19749,11 +19763,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="O2">
+            <xdr:cNvPr id="23" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8EC450C-D03B-AB94-CF2B-93294EFB52D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{860E777E-9852-7E96-E0C5-6CDBFC96BC88}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19801,11 +19815,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="VF">
+            <xdr:cNvPr id="24" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EB87D17-6594-FADE-42FC-D92315D5B584}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34E6A4F6-6D0A-8600-7893-78C96A7FCD68}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19853,11 +19867,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="EM">
+            <xdr:cNvPr id="25" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2900B20A-99F0-A6A4-0C63-5D1B33A85707}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124576A9-1CBF-DF0F-5085-591174913DD4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19905,11 +19919,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="RC">
+            <xdr:cNvPr id="26" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D90E84BE-804D-5DFF-FD02-4340C6BB706C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{649227EA-89F7-40AB-7B8C-7DC713A7C6E0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -19957,11 +19971,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="PP">
+            <xdr:cNvPr id="27" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7F595E6-C3CC-0316-8959-54D11D984BA9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2171877E-5F86-67E4-4F88-5F5A25433857}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20009,11 +20023,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="EN">
+            <xdr:cNvPr id="28" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1E2A28-6756-691D-31BA-FC4F5266C445}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBABEB11-7BF6-7D62-929D-3906B7A35E3A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20061,11 +20075,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="32" name="CL">
+            <xdr:cNvPr id="29" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E4B3F71-D900-BC69-6B52-CE1D0286EBDC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5801B3CD-3183-71F2-FF62-2B8BD3AA45D6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20191,10 +20205,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="MENU">
+        <xdr:cNvPr id="15" name="MENU">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6022C338-6B42-4ECB-9AE2-B2638E24CF4F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E255BB8-F51D-403F-A974-ECF978A33FCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20210,10 +20224,10 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="FONDO BLANCO">
+          <xdr:cNvPr id="16" name="FONDO BLANCO">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC0BD42A-D9C5-3934-AC8B-68D944E077DC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AD908CA-942C-09E1-24AB-B6F8EE73D1D0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -20261,10 +20275,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="FTP-MOODLE">
+          <xdr:cNvPr id="17" name="FTP-MOODLE">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F97CA11-2669-A5AF-174B-9682D249D17F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D3EA76F-BCFF-F459-43EA-03765EED9046}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -20280,10 +20294,10 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="33" name="Moodle">
+            <xdr:cNvPr id="30" name="Moodle">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC2AD54-91FE-9620-8C7B-1206930494F5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{490CECE3-3988-E1A6-051C-0615B834EBB5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20308,10 +20322,10 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="34" name="FTP">
+            <xdr:cNvPr id="31" name="FTP">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3F1DB80-C740-CACA-B01E-9438F2C6C4A3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EE94A2-ECFF-92F7-07D0-FDF48B30ED21}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20337,11 +20351,11 @@
       </xdr:grpSp>
       <xdr:sp macro="[0]!IR_DICCIONARIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="DICCIONARIO">
+          <xdr:cNvPr id="18" name="DICCIONARIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="DICTIONARY"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E0E825F-75C9-DAAC-C7FD-428F59F39E5D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F106A641-C3D3-1DD9-01B4-09FB4B6C7752}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -20389,11 +20403,11 @@
       </xdr:sp>
       <xdr:sp macro="[0]!IR_INICIO" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="INICIO">
+          <xdr:cNvPr id="20" name="INICIO">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="INICIO / HOME"/>
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C6C628-0F34-8FE8-D656-6496392BC373}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6968AC27-51D2-6879-4B59-F9FE3ECAE025}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -20441,10 +20455,10 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="TIPO PREGUNTAS">
+          <xdr:cNvPr id="21" name="TIPO PREGUNTAS">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1C376A-CAB8-F1D3-6FA9-88CE54E638CD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B9EA2E1-0A51-B056-1CA5-BCCA60AE6789}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -20460,11 +20474,11 @@
         </xdr:grpSpPr>
         <xdr:sp macro="[0]!IR_OM" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="OM">
+            <xdr:cNvPr id="22" name="OM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7" tooltip="OM 1R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CE3E6F5-FA43-C708-E809-D1E9B1616C64}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3447CDF-0A53-305E-6D4E-8043D8818B78}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20512,11 +20526,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_O2" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="O2">
+            <xdr:cNvPr id="23" name="O2">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8" tooltip="OM +R"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECFA2221-BCF7-7AA2-BC40-F08C52088184}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{068B4F22-B0EA-FB87-CD6F-763C131B57D7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20564,11 +20578,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_VF" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="VF">
+            <xdr:cNvPr id="24" name="VF">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9" tooltip="VF"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4C0ECEF-72E9-4674-BD32-5103591F5524}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED542926-EEC1-E730-B2B8-E7B63E3F5206}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20616,11 +20630,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_E" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="EM">
+            <xdr:cNvPr id="25" name="EM">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10" tooltip="EM"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27F8860E-E4EE-07C4-1DC7-62A78037C11B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04040878-D364-7D27-85D6-8B52DC1EDA55}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20668,11 +20682,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_RC" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="RC">
+            <xdr:cNvPr id="26" name="RC">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11" tooltip="RC"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0685B877-0901-B970-100F-87B3CCB19670}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D412B3DA-E6A6-C25C-071A-5B3219055381}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20720,11 +20734,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_PP" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="PP">
+            <xdr:cNvPr id="27" name="PP">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tooltip="PP"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29992A27-FC30-0B4C-B7BF-5900243940BB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10B177F0-76B9-64B2-E7B3-1F17181AE26F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20772,11 +20786,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_EN" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="EN">
+            <xdr:cNvPr id="28" name="EN">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tooltip="EN"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B940083-3931-23D1-928F-016721FEFBD4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49FAD67B-870F-3BEF-7EC9-326C59242C95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20824,11 +20838,11 @@
         </xdr:sp>
         <xdr:sp macro="[0]!IR_CL" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="CL">
+            <xdr:cNvPr id="29" name="CL">
               <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14" tooltip="CL"/>
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9F202F-6698-B021-7555-771106BCC2FA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C3AA3A-490E-A98A-9459-324593FEDAF6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -20920,7 +20934,6 @@
       <sheetName val="DOC_2"/>
       <sheetName val="DOC_TEMP"/>
       <sheetName val="OCA"/>
-      <sheetName val="FastTest PlugIn"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -20955,7 +20968,6 @@
       <sheetData sheetId="29"/>
       <sheetData sheetId="30"/>
       <sheetData sheetId="31"/>
-      <sheetData sheetId="32" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -20976,54 +20988,54 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla_Menu" displayName="Tabla_Menu" ref="S2:AF30" totalsRowCount="1" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla_Menu" displayName="Tabla_Menu" ref="S2:AF30" totalsRowCount="1" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="S2:AF29" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="N Sub" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="N Sub" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="41">
       <calculatedColumnFormula>IF(Tabla_Menu[[#This Row],[Nivel]]=T2,0,COUNTIF(Tabla_Menu[Nivel],Tabla_Menu[[#This Row],[Nivel]]))</calculatedColumnFormula>
       <totalsRowFormula>COUNTIF(Tabla_Menu[N Sub],"&lt;&gt;0")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Nivel" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Nivel" dataDxfId="40" totalsRowDxfId="39">
       <calculatedColumnFormula>IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Nombre" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Nombre" dataDxfId="38" totalsRowDxfId="37">
       <calculatedColumnFormula>IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="On Action" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Face Id" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Begin Group" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Nivel 1" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Nivel 2" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Teclas" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="HOJAS NO MUESTRA" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="N/A" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="On Action" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Face Id" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Begin Group" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Nivel 1" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Nivel 2" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Teclas" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="HOJAS NO MUESTRA" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="N/A" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>IF(OR(Tabla_Menu[[#This Row],[Nivel]]="",IFERROR(SEARCH(MID(CELL("nombrearchivo"),FIND(".xlsm]",CELL("nombrearchivo"),1)+6,100),Tabla_Menu[[#This Row],[HOJAS NO MUESTRA]],1),0)&gt;0),"N/A","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="Num N/A" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="Num N/A" dataDxfId="20" totalsRowDxfId="19">
       <calculatedColumnFormula>IF(Tabla_Menu[[#This Row],[N/A]]="",,COUNTIF(Tabla_Menu[Nivel &amp; Incluir],Tabla_Menu[[#This Row],[Nivel &amp; Incluir]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Nivel &amp; Incluir" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="Nivel &amp; Incluir" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="[Teclas]" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="[Teclas]" dataDxfId="16" totalsRowDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Tabla_UCA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla_Comandos" displayName="Tabla_Comandos" ref="U37:W44" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla_Comandos" displayName="Tabla_Comandos" ref="U37:W44" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="11" tableBorderDxfId="12">
   <autoFilter ref="U37:W43" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="CommandBars" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="CommandBars" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
       <totalsRowFormula>COUNTA(Tabla_Comandos[CommandBars])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Cambio" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Activa/Des" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Cambio" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Activa/Des" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21309,88 +21321,88 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabla_EN" displayName="Tabla_EN" ref="A4:AI6" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabla_EN" displayName="Tabla_EN" ref="A4:AI6" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="A4:AI6" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="35">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="C1" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="C2" dataDxfId="114"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Columna1" dataDxfId="113"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Columna2" dataDxfId="112"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Descripción" dataDxfId="111"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="FastTest PlugIn - ENSAYO_x000a__x000a_Enunciado de la pregunta" dataDxfId="110"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Formato de la Respuesta_x000a_Requerir texto" dataDxfId="109"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Requerir texto" dataDxfId="108"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Tamaño de la caja de entrada" dataDxfId="107"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Permitir archivos adjuntos" dataDxfId="106"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Archivos adjuntos requeridos" dataDxfId="105"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Plantilla de Respuesta" dataDxfId="104"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Información para el evaluador" dataDxfId="103"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="Columna3" dataDxfId="102"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Columna4" dataDxfId="101"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Columna5" dataDxfId="100"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Columna6" dataDxfId="99"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Columna7" dataDxfId="98"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0700-000013000000}" name="Columna8" dataDxfId="97"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0700-000014000000}" name="Columna9" dataDxfId="96"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0700-000015000000}" name="Columna10" dataDxfId="95"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0700-000016000000}" name="Columna11" dataDxfId="94"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0700-000017000000}" name="Columna12" dataDxfId="93"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0700-000018000000}" name="Columna13" dataDxfId="92"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0700-000019000000}" name="Columna14" dataDxfId="91"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0700-00001A000000}" name="Columna15" dataDxfId="90"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0700-00001B000000}" name="Columna16" dataDxfId="89"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0700-00001C000000}" name="Columna17" dataDxfId="88"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0700-00001D000000}" name="Columna18" dataDxfId="87"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0700-00001E000000}" name="Columna19" dataDxfId="86"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0700-00001F000000}" name="Columna20" dataDxfId="85"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0700-000020000000}" name="Columna21" dataDxfId="84"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0700-000021000000}" name="Columna22" dataDxfId="83"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0700-000022000000}" name="Columna23" dataDxfId="82"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0700-000023000000}" name="Imagen" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="C1" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="C2" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Columna1" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Columna2" dataDxfId="114"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Descripción" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="FastTest PlugIn - ENSAYO_x000a__x000a_Enunciado de la pregunta" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Formato de la Respuesta_x000a_Requerir texto" dataDxfId="111"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Requerir texto" dataDxfId="110"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Tamaño de la caja de entrada" dataDxfId="109"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Permitir archivos adjuntos" dataDxfId="108"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Archivos adjuntos requeridos" dataDxfId="107"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Plantilla de Respuesta" dataDxfId="106"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Información para el evaluador" dataDxfId="105"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="Columna3" dataDxfId="104"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Columna4" dataDxfId="103"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Columna5" dataDxfId="102"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Columna6" dataDxfId="101"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Columna7" dataDxfId="100"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0700-000013000000}" name="Columna8" dataDxfId="99"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0700-000014000000}" name="Columna9" dataDxfId="98"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0700-000015000000}" name="Columna10" dataDxfId="97"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0700-000016000000}" name="Columna11" dataDxfId="96"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0700-000017000000}" name="Columna12" dataDxfId="95"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0700-000018000000}" name="Columna13" dataDxfId="94"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0700-000019000000}" name="Columna14" dataDxfId="93"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0700-00001A000000}" name="Columna15" dataDxfId="92"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0700-00001B000000}" name="Columna16" dataDxfId="91"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0700-00001C000000}" name="Columna17" dataDxfId="90"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0700-00001D000000}" name="Columna18" dataDxfId="89"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0700-00001E000000}" name="Columna19" dataDxfId="88"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0700-00001F000000}" name="Columna20" dataDxfId="87"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0700-000020000000}" name="Columna21" dataDxfId="86"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0700-000021000000}" name="Columna22" dataDxfId="85"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0700-000022000000}" name="Columna23" dataDxfId="84"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0700-000023000000}" name="Imagen" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla_CL" displayName="Tabla_CL" ref="A4:AI5" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
-  <autoFilter ref="A4:AI5" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla_CL" displayName="Tabla_CL" ref="A4:AI7" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+  <autoFilter ref="A4:AI7" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="35">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="C1" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="C2" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Columna1" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Columna2" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Descripcion" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Enunciado" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Ancho RC" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Columna3" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Ancho IM" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Columna5" dataDxfId="69"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Columna6" dataDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Columna7" dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="Columna8" dataDxfId="66"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="Columna9" dataDxfId="65"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Columna10" dataDxfId="64"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Columna11" dataDxfId="63"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Columna12" dataDxfId="62"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Columna13" dataDxfId="61"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0800-000013000000}" name="Columna14" dataDxfId="60"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0800-000014000000}" name="Columna15" dataDxfId="59"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0800-000015000000}" name="Columna16" dataDxfId="58"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0800-000016000000}" name="Columna17" dataDxfId="57"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0800-000017000000}" name="Columna18" dataDxfId="56"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0800-000018000000}" name="Columna19" dataDxfId="55"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0800-000019000000}" name="Columna20" dataDxfId="54"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0800-00001A000000}" name="Columna21" dataDxfId="53"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0800-00001B000000}" name="Columna22" dataDxfId="52"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0800-00001C000000}" name="Columna23" dataDxfId="51"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0800-00001D000000}" name="Columna24" dataDxfId="50"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0800-00001E000000}" name="Columna25" dataDxfId="49"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0800-00001F000000}" name="Pista 1" dataDxfId="48"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0800-000020000000}" name="Pista 2" dataDxfId="47"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0800-000021000000}" name="Pista 3" dataDxfId="46"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0800-000022000000}" name="Pista 4" dataDxfId="45"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0800-000023000000}" name="Imagen" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="C1" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="C2" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Columna1" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Columna2" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Descripcion" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Enunciado" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Ancho RC" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Columna3" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Ancho IM" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Columna5" dataDxfId="71"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Columna6" dataDxfId="70"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="Columna7" dataDxfId="69"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="Columna8" dataDxfId="68"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="Columna9" dataDxfId="67"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Columna10" dataDxfId="66"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Columna11" dataDxfId="65"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Columna12" dataDxfId="64"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Columna13" dataDxfId="63"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0800-000013000000}" name="Columna14" dataDxfId="62"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0800-000014000000}" name="Columna15" dataDxfId="61"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0800-000015000000}" name="Columna16" dataDxfId="60"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0800-000016000000}" name="Columna17" dataDxfId="59"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0800-000017000000}" name="Columna18" dataDxfId="58"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0800-000018000000}" name="Columna19" dataDxfId="57"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0800-000019000000}" name="Columna20" dataDxfId="56"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0800-00001A000000}" name="Columna21" dataDxfId="55"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0800-00001B000000}" name="Columna22" dataDxfId="54"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0800-00001C000000}" name="Columna23" dataDxfId="53"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0800-00001D000000}" name="Columna24" dataDxfId="52"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0800-00001E000000}" name="Columna25" dataDxfId="51"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0800-00001F000000}" name="Pista 1" dataDxfId="50"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0800-000020000000}" name="Pista 2" dataDxfId="49"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0800-000021000000}" name="Pista 3" dataDxfId="48"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0800-000022000000}" name="Pista 4" dataDxfId="47"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0800-000023000000}" name="Imagen" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -21662,14 +21674,14 @@
   <sheetPr codeName="Hoja_00"/>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="116" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
       <pane xSplit="19" ySplit="46" topLeftCell="T47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
-      <selection pane="bottomRight" sqref="A1:A9"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" zeroHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10.64453125" customWidth="1"/>
     <col min="2" max="2" width="2.64453125" customWidth="1"/>
@@ -21733,7 +21745,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="269" t="str">
         <f ca="1">INDIRECT("Z_IN_04_"&amp;IDIOMA)</f>
-        <v>Esta Aplicación ha sido desarrollada, en la primera versión, por:</v>
+        <v>This Application has been developed, in the first version, by:</v>
       </c>
       <c r="H3" s="269"/>
       <c r="I3" s="269"/>
@@ -21812,7 +21824,7 @@
       <c r="O6" s="244"/>
       <c r="P6" s="272" t="str">
         <f ca="1">INDIRECT("Z_IN_01_"&amp;IDIOMA)</f>
-        <v>CANAL YOUTUBE</v>
+        <v>YOUTUBE CHANNEL</v>
       </c>
       <c r="Q6" s="272"/>
       <c r="R6" s="272"/>
@@ -21829,7 +21841,7 @@
       <c r="H7" s="134"/>
       <c r="I7" s="269" t="str">
         <f ca="1">INDIRECT("Z_IN_05_"&amp;IDIOMA)</f>
-        <v>Universidad de Cádiz</v>
+        <v>Cadiz University</v>
       </c>
       <c r="J7" s="269"/>
       <c r="K7" s="269"/>
@@ -21868,7 +21880,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="255" t="str">
         <f ca="1">INDIRECT("Z_IN_03_"&amp;IDIOMA)</f>
-        <v>LEER CON ATENCIÓN</v>
+        <v>READ CAREFULLY</v>
       </c>
       <c r="D9" s="255"/>
       <c r="E9" s="5"/>
@@ -21913,16 +21925,16 @@
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="265" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="256" t="str">
         <f ca="1">INDIRECT("Z_IN_06_"&amp;IDIOMA)</f>
-        <v>1. Esta aplicación se ha desarrollado gracias a un Proyecto de Innovación Docente aprobado por la Unidad de Innovación Docente de la Universidad de Cádiz.
-2. El usuario final es aquel docente que quiera usar los CUESTIONARIOS de la plataforma Moodle. También la puede usar quien quiera tener sus Bancos de Preguntas almacenados en un mismo sitio y con orden.
-3. La aplicación sirve para facilitar la creación de un BANCO DE PREGUNTAS para los cuestionarios, el usuario final deberá repasar que las preguntas se importan bien (al menos las primeras veces) así como si ha rellenado los datos de manera adecuada, como si lo estuviera haciendo en Moodle.
-Pulsa sobre el TIPO DE PREGUNTA sobre el que quieres CONSULTAR las preguntas almacenadas.</v>
+        <v>1. This application has been developed thanks to a Teaching Innovation Project approved by the Teaching Innovation Unit of the University of Cádiz.
+2. The end user is the teacher who wants to use the QUESTIONNAIRES of the Moodle platform. It can also be used by anyone who wants to have their Question Banks stored in one place and in order.
+3. The application serves to facilitate the creation of a BANK OF QUESTIONS for the questionnaires, the end user must check that the questions are imported correctly (at least the first times) as well as if they have filled in the data appropriately, as if was doing in Moodle.
+Click on the TYPE OF QUESTION on which you want to CONSULT the stored questions.</v>
       </c>
       <c r="E11" s="256"/>
       <c r="F11" s="256"/>
@@ -22045,7 +22057,7 @@
     <row r="17" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A17" s="266" t="str">
         <f>IFERROR(HLOOKUP(LANGUAGE,DICCIONARIO!F1:K20,20,0),LANGUAGE)</f>
-        <v>PERSONALIZAR DICCIONARIO</v>
+        <v>CUSTOM DICTIONARY</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -22172,37 +22184,37 @@
       <c r="B23" s="4"/>
       <c r="C23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_10_"&amp;IDIOMA)</f>
-        <v>OM 1R</v>
+        <v>MC 1A</v>
       </c>
       <c r="D23" s="258"/>
       <c r="E23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_11_"&amp;IDIOMA)</f>
-        <v>OM +R</v>
+        <v>MC +A</v>
       </c>
       <c r="F23" s="259"/>
       <c r="G23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_12_"&amp;IDIOMA)</f>
-        <v>VF</v>
+        <v>TF</v>
       </c>
       <c r="H23" s="259"/>
       <c r="I23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_13_"&amp;IDIOMA)</f>
-        <v>EM</v>
+        <v>MA</v>
       </c>
       <c r="J23" s="258"/>
       <c r="K23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_14_"&amp;IDIOMA)</f>
-        <v>RC</v>
+        <v>SA</v>
       </c>
       <c r="L23" s="259"/>
       <c r="M23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_15_"&amp;IDIOMA)</f>
-        <v>PP</v>
+        <v>MW</v>
       </c>
       <c r="N23" s="259"/>
       <c r="O23" s="257" t="str">
         <f ca="1">INDIRECT("Z_BP_31_"&amp;IDIOMA)</f>
-        <v>EN</v>
+        <v>ES</v>
       </c>
       <c r="P23" s="259"/>
       <c r="Q23" s="257" t="str">
@@ -22216,37 +22228,37 @@
       <c r="B24" s="4"/>
       <c r="C24" s="248" t="str">
         <f ca="1">INDIRECT("Z_IN_08_"&amp;IDIOMA)</f>
-        <v xml:space="preserve">Opción Múltiple 1R </v>
+        <v>Multiple Choice 1A</v>
       </c>
       <c r="D24" s="249"/>
       <c r="E24" s="249" t="str">
         <f ca="1">INDIRECT("Z_IN_09_"&amp;IDIOMA)</f>
-        <v xml:space="preserve">Opción Múltiple +R </v>
+        <v>Multiple Choice +A</v>
       </c>
       <c r="F24" s="249"/>
       <c r="G24" s="249" t="str">
         <f ca="1">INDIRECT("Z_IN_10_"&amp;IDIOMA)</f>
-        <v>Verdadero/Falso</v>
+        <v>True/False</v>
       </c>
       <c r="H24" s="249"/>
       <c r="I24" s="249" t="str">
         <f ca="1">INDIRECT("Z_IN_11_"&amp;IDIOMA)</f>
-        <v>Emparejar</v>
+        <v>Matching</v>
       </c>
       <c r="J24" s="249"/>
       <c r="K24" s="249" t="str">
         <f ca="1">INDIRECT("Z_IN_12_"&amp;IDIOMA)</f>
-        <v>Respuesta Corta</v>
+        <v>Short Answer</v>
       </c>
       <c r="L24" s="249"/>
       <c r="M24" s="249" t="str">
         <f ca="1">INDIRECT("Z_IN_13_"&amp;IDIOMA)</f>
-        <v>Palabra Perdida</v>
+        <v>Missing Word</v>
       </c>
       <c r="N24" s="249"/>
       <c r="O24" s="249" t="str">
         <f ca="1">INDIRECT("Z_IN_16_"&amp;IDIOMA)</f>
-        <v>Ensayo</v>
+        <v>Essay</v>
       </c>
       <c r="P24" s="249"/>
       <c r="Q24" s="249" t="str">
@@ -22280,42 +22292,42 @@
       <c r="B26" s="4"/>
       <c r="C26" s="245" t="str">
         <f ca="1">'Datos OM'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>3 Preguntas</v>
+        <v>3 Questions</v>
       </c>
       <c r="D26" s="247"/>
       <c r="E26" s="245" t="str">
         <f ca="1">'Datos O2'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>2 Preguntas</v>
+        <v>2 Questions</v>
       </c>
       <c r="F26" s="246"/>
       <c r="G26" s="245" t="str">
         <f ca="1">'Datos VF'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>2 Preguntas</v>
+        <v>2 Questions</v>
       </c>
       <c r="H26" s="246"/>
       <c r="I26" s="245" t="str">
         <f ca="1">'Datos EM'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>3 Preguntas</v>
+        <v>3 Questions</v>
       </c>
       <c r="J26" s="247"/>
       <c r="K26" s="245" t="str">
         <f ca="1">'Datos RC'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>2 Preguntas</v>
+        <v>2 Questions</v>
       </c>
       <c r="L26" s="246"/>
       <c r="M26" s="245" t="str">
         <f ca="1">'Datos PP'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>2 Preguntas</v>
+        <v>2 Questions</v>
       </c>
       <c r="N26" s="246"/>
       <c r="O26" s="245" t="str">
         <f ca="1">'Datos EN'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>2 Preguntas</v>
+        <v>2 Questions</v>
       </c>
       <c r="P26" s="246"/>
       <c r="Q26" s="245" t="str">
         <f ca="1">'Datos CL'!G2&amp;" "&amp;INDIRECT("Z_IN_15_"&amp;IDIOMA)</f>
-        <v>1 Preguntas</v>
+        <v>3 Questions</v>
       </c>
       <c r="R26" s="246"/>
       <c r="S26" s="6"/>
@@ -22325,7 +22337,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="267" t="str">
         <f ca="1">INDIRECT("Z_IN_07_"&amp;IDIOMA)</f>
-        <v>Esta HOJA sirve para almacenar las preguntas y poder reutilizarlas cuando sea necesario, sin tener que volver a escribirlas para un nuevo BANCO DE PREGUNTAS.</v>
+        <v>This SHEET is used to store the questions and to be able to reuse them when necessary, without having to retype them for a new BANK OF QUESTIONS.</v>
       </c>
       <c r="E27" s="267"/>
       <c r="F27" s="267"/>
@@ -22511,7 +22523,7 @@
     <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.5">
       <c r="A37" s="37" t="str">
         <f>IFERROR(VLOOKUP(LANGUAGE,Tabla_ID[],2,0),"")</f>
-        <v>S</v>
+        <v>E</v>
       </c>
       <c r="F37" s="242">
         <v>6</v>
@@ -22587,7 +22599,7 @@
     <row r="46" spans="1:19" ht="15" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="40" t="str">
         <f>A17</f>
-        <v>PERSONALIZAR DICCIONARIO</v>
+        <v>CUSTOM DICTIONARY</v>
       </c>
       <c r="B46" s="43" t="s">
         <v>388</v>
@@ -22595,7 +22607,7 @@
     </row>
     <row r="47" spans="1:19" ht="5.0999999999999996" customHeight="1" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="B4ZtyPI8lv6/MGOS3+9a5fUlVKn8W7m5tc5qom7GwcpKDO4mxFaT3Eq647jn8+lsT+zoaLPf06hAUqFkuo98DA==" saltValue="Oavj1BI2LOGiAwJ94csGEA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="42">
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="A11:A13"/>
@@ -22672,7 +22684,7 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" zeroHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" zeroHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10.64453125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="3" width="6" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -22712,11 +22724,11 @@
       <c r="C1" s="45"/>
       <c r="D1" s="141" t="str">
         <f ca="1">INDIRECT("Z_IN_00_"&amp;IDIOMA)</f>
-        <v>INICIO</v>
+        <v>HOME</v>
       </c>
       <c r="E1" s="34" t="str">
         <f>LANGUAGE</f>
-        <v>ESPAÑOL</v>
+        <v>ENGLISH</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>12</v>
@@ -22811,11 +22823,11 @@
       <c r="C2" s="44"/>
       <c r="D2" s="142" t="str">
         <f>"LINK "&amp;INICIO!A46</f>
-        <v>LINK PERSONALIZAR DICCIONARIO</v>
+        <v>LINK CUSTOM DICTIONARY</v>
       </c>
       <c r="E2" s="35" t="str">
         <f>IFERROR(INDEX(F2:K20,1,MATCH(E1,F20:K20,0)),IDIOMA)</f>
-        <v>S</v>
+        <v>E</v>
       </c>
       <c r="F2" s="47" t="s">
         <v>13</v>
@@ -22889,7 +22901,7 @@
       </c>
       <c r="AI2" s="190" t="str">
         <f>IF(IDIOMA="S","May","Shift")&amp;"+"</f>
-        <v>May+</v>
+        <v>Shift+</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -22906,7 +22918,7 @@
       <c r="D3" s="168"/>
       <c r="E3" s="146" t="str">
         <f>IFERROR(IF(D3&lt;&gt;"",D3,HLOOKUP($E$2,$F$2:K3,ROW(D3)-1,0)),F3)</f>
-        <v>INICIO</v>
+        <v>HOME</v>
       </c>
       <c r="F3" s="146" t="s">
         <v>11</v>
@@ -22951,11 +22963,11 @@
       </c>
       <c r="T3" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>MENU EXCEL</v>
+        <v>EXCEL MENU</v>
       </c>
       <c r="U3" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">MENU EXCEL </v>
+        <v xml:space="preserve">EXCEL MENU </v>
       </c>
       <c r="V3" s="191" t="s">
         <v>650</v>
@@ -22988,7 +23000,7 @@
       </c>
       <c r="AE3" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>MENU EXCEL</v>
+        <v>EXCEL MENU</v>
       </c>
       <c r="AF3" s="179"/>
     </row>
@@ -23007,7 +23019,7 @@
       <c r="D4" s="198"/>
       <c r="E4" s="149" t="str">
         <f>IFERROR(IF(D4&lt;&gt;"",D4,HLOOKUP($E$2,$F$2:K4,ROW(D4)-1,0)),F4)</f>
-        <v>CANAL YOUTUBE</v>
+        <v>YOUTUBE CHANNEL</v>
       </c>
       <c r="F4" s="147" t="s">
         <v>403</v>
@@ -23048,11 +23060,11 @@
       </c>
       <c r="T4" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="U4" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">GUARDAR  </v>
+        <v xml:space="preserve">SAVE </v>
       </c>
       <c r="V4" s="191" t="s">
         <v>489</v>
@@ -23083,7 +23095,7 @@
       </c>
       <c r="AE4" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="AF4" s="179"/>
     </row>
@@ -23102,10 +23114,10 @@
       <c r="D5" s="170"/>
       <c r="E5" s="148" t="str">
         <f>IFERROR(IF(D5&lt;&gt;"",D5,HLOOKUP($E$2,$F$2:K5,ROW(D5)-1,0)),F5)</f>
-        <v>NO FUNCIONA CON
-VERSIONES DE EXCEL 
-ANTERIORES A 2007
-NI CON LA ÚLTIMA ACTUALIZACIÓN DE MAC</v>
+        <v xml:space="preserve">DOES NOT WORK WITH
+EXCEL VERSIONS
+BEFORE 2007
+NOT WITH THE LATEST MAC UPDATE </v>
       </c>
       <c r="F5" s="148" t="s">
         <v>34</v>
@@ -23150,11 +23162,11 @@
       </c>
       <c r="T5" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="U5" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">CERRAR </v>
+        <v xml:space="preserve">CLOSE </v>
       </c>
       <c r="V5" s="191" t="s">
         <v>493</v>
@@ -23185,7 +23197,7 @@
       </c>
       <c r="AE5" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="AF5" s="179"/>
     </row>
@@ -23204,7 +23216,7 @@
       <c r="D6" s="169"/>
       <c r="E6" s="147" t="str">
         <f>IFERROR(IF(D6&lt;&gt;"",D6,HLOOKUP($E$2,$F$2:K6,ROW(D6)-1,0)),F6)</f>
-        <v>LEER CON ATENCIÓN</v>
+        <v>READ CAREFULLY</v>
       </c>
       <c r="F6" s="147" t="s">
         <v>2</v>
@@ -23249,11 +23261,11 @@
       </c>
       <c r="T6" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="U6" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">COPIAR </v>
+        <v xml:space="preserve">COPY </v>
       </c>
       <c r="V6" s="191" t="s">
         <v>495</v>
@@ -23286,7 +23298,7 @@
       </c>
       <c r="AE6" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="AF6" s="179"/>
     </row>
@@ -23305,7 +23317,7 @@
       <c r="D7" s="170"/>
       <c r="E7" s="148" t="str">
         <f>IFERROR(IF(D7&lt;&gt;"",D7,HLOOKUP($E$2,$F$2:K7,ROW(D7)-1,0)),F7)</f>
-        <v>Esta Aplicación ha sido desarrollada, en la primera versión, por:</v>
+        <v>This Application has been developed, in the first version, by:</v>
       </c>
       <c r="F7" s="148" t="s">
         <v>4</v>
@@ -23350,11 +23362,11 @@
       </c>
       <c r="T7" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="U7" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">PEGAR </v>
+        <v xml:space="preserve">PASTE </v>
       </c>
       <c r="V7" s="191" t="s">
         <v>497</v>
@@ -23387,7 +23399,7 @@
       </c>
       <c r="AE7" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="AF7" s="179"/>
     </row>
@@ -23406,7 +23418,7 @@
       <c r="D8" s="169"/>
       <c r="E8" s="147" t="str">
         <f>IFERROR(IF(D8&lt;&gt;"",D8,HLOOKUP($E$2,$F$2:K8,ROW(D8)-1,0)),F8)</f>
-        <v>Universidad de Cádiz</v>
+        <v>Cadiz University</v>
       </c>
       <c r="F8" s="147" t="s">
         <v>1</v>
@@ -23451,11 +23463,11 @@
       </c>
       <c r="T8" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U8" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">INICIO </v>
+        <v xml:space="preserve">HOME </v>
       </c>
       <c r="V8" s="191" t="s">
         <v>499</v>
@@ -23488,7 +23500,7 @@
       </c>
       <c r="AE8" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF8" s="179"/>
     </row>
@@ -23507,10 +23519,10 @@
       <c r="D9" s="170"/>
       <c r="E9" s="148" t="str">
         <f>IFERROR(IF(D9&lt;&gt;"",D9,HLOOKUP($E$2,$F$2:K9,ROW(D9)-1,0)),F9)</f>
-        <v>1. Esta aplicación se ha desarrollado gracias a un Proyecto de Innovación Docente aprobado por la Unidad de Innovación Docente de la Universidad de Cádiz.
-2. El usuario final es aquel docente que quiera usar los CUESTIONARIOS de la plataforma Moodle. También la puede usar quien quiera tener sus Bancos de Preguntas almacenados en un mismo sitio y con orden.
-3. La aplicación sirve para facilitar la creación de un BANCO DE PREGUNTAS para los cuestionarios, el usuario final deberá repasar que las preguntas se importan bien (al menos las primeras veces) así como si ha rellenado los datos de manera adecuada, como si lo estuviera haciendo en Moodle.
-Pulsa sobre el TIPO DE PREGUNTA sobre el que quieres CONSULTAR las preguntas almacenadas.</v>
+        <v>1. This application has been developed thanks to a Teaching Innovation Project approved by the Teaching Innovation Unit of the University of Cádiz.
+2. The end user is the teacher who wants to use the QUESTIONNAIRES of the Moodle platform. It can also be used by anyone who wants to have their Question Banks stored in one place and in order.
+3. The application serves to facilitate the creation of a BANK OF QUESTIONS for the questionnaires, the end user must check that the questions are imported correctly (at least the first times) as well as if they have filled in the data appropriately, as if was doing in Moodle.
+Click on the TYPE OF QUESTION on which you want to CONSULT the stored questions.</v>
       </c>
       <c r="F9" s="148" t="s">
         <v>59</v>
@@ -23555,11 +23567,11 @@
       </c>
       <c r="T9" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U9" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">DICCIONARIO </v>
+        <v xml:space="preserve">DICTIONARY </v>
       </c>
       <c r="V9" s="191" t="s">
         <v>502</v>
@@ -23592,7 +23604,7 @@
       </c>
       <c r="AE9" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF9" s="179"/>
     </row>
@@ -23611,7 +23623,7 @@
       <c r="D10" s="169"/>
       <c r="E10" s="147" t="str">
         <f>IFERROR(IF(D10&lt;&gt;"",D10,HLOOKUP($E$2,$F$2:K10,ROW(D10)-1,0)),F10)</f>
-        <v>Esta HOJA sirve para almacenar las preguntas y poder reutilizarlas cuando sea necesario, sin tener que volver a escribirlas para un nuevo BANCO DE PREGUNTAS.</v>
+        <v>This SHEET is used to store the questions and to be able to reuse them when necessary, without having to retype them for a new BANK OF QUESTIONS.</v>
       </c>
       <c r="F10" s="147" t="s">
         <v>381</v>
@@ -23656,11 +23668,11 @@
       </c>
       <c r="T10" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U10" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Opción Múltiple 1R  </v>
+        <v xml:space="preserve">Multiple Choice 1A </v>
       </c>
       <c r="V10" s="191" t="s">
         <v>570</v>
@@ -23693,7 +23705,7 @@
       </c>
       <c r="AE10" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF10" s="179"/>
     </row>
@@ -23712,7 +23724,7 @@
       <c r="D11" s="170"/>
       <c r="E11" s="148" t="str">
         <f>IFERROR(IF(D11&lt;&gt;"",D11,HLOOKUP($E$2,$F$2:K11,ROW(D11)-1,0)),F11)</f>
-        <v xml:space="preserve">Opción Múltiple 1R </v>
+        <v>Multiple Choice 1A</v>
       </c>
       <c r="F11" s="148" t="s">
         <v>67</v>
@@ -23757,11 +23769,11 @@
       </c>
       <c r="T11" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U11" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Opción Múltiple +R  </v>
+        <v xml:space="preserve">Multiple Choice +A </v>
       </c>
       <c r="V11" s="191" t="s">
         <v>571</v>
@@ -23794,7 +23806,7 @@
       </c>
       <c r="AE11" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF11" s="179"/>
     </row>
@@ -23813,7 +23825,7 @@
       <c r="D12" s="169"/>
       <c r="E12" s="147" t="str">
         <f>IFERROR(IF(D12&lt;&gt;"",D12,HLOOKUP($E$2,$F$2:K12,ROW(D12)-1,0)),F12)</f>
-        <v xml:space="preserve">Opción Múltiple +R </v>
+        <v>Multiple Choice +A</v>
       </c>
       <c r="F12" s="147" t="s">
         <v>451</v>
@@ -23858,11 +23870,11 @@
       </c>
       <c r="T12" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U12" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Verdadero/Falso </v>
+        <v xml:space="preserve">True/False </v>
       </c>
       <c r="V12" s="191" t="s">
         <v>572</v>
@@ -23895,7 +23907,7 @@
       </c>
       <c r="AE12" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF12" s="179"/>
     </row>
@@ -23914,7 +23926,7 @@
       <c r="D13" s="170"/>
       <c r="E13" s="148" t="str">
         <f>IFERROR(IF(D13&lt;&gt;"",D13,HLOOKUP($E$2,$F$2:K13,ROW(D13)-1,0)),F13)</f>
-        <v>Verdadero/Falso</v>
+        <v>True/False</v>
       </c>
       <c r="F13" s="148" t="s">
         <v>457</v>
@@ -23959,11 +23971,11 @@
       </c>
       <c r="T13" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U13" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Emparejar </v>
+        <v xml:space="preserve">Matching </v>
       </c>
       <c r="V13" s="191" t="s">
         <v>587</v>
@@ -23996,7 +24008,7 @@
       </c>
       <c r="AE13" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF13" s="179"/>
     </row>
@@ -24015,7 +24027,7 @@
       <c r="D14" s="169"/>
       <c r="E14" s="147" t="str">
         <f>IFERROR(IF(D14&lt;&gt;"",D14,HLOOKUP($E$2,$F$2:K14,ROW(D14)-1,0)),F14)</f>
-        <v>Emparejar</v>
+        <v>Matching</v>
       </c>
       <c r="F14" s="147" t="s">
         <v>7</v>
@@ -24060,11 +24072,11 @@
       </c>
       <c r="T14" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U14" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Respuesta Corta </v>
+        <v xml:space="preserve">Short Answer </v>
       </c>
       <c r="V14" s="191" t="s">
         <v>573</v>
@@ -24097,7 +24109,7 @@
       </c>
       <c r="AE14" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF14" s="179"/>
     </row>
@@ -24116,7 +24128,7 @@
       <c r="D15" s="170"/>
       <c r="E15" s="148" t="str">
         <f>IFERROR(IF(D15&lt;&gt;"",D15,HLOOKUP($E$2,$F$2:K15,ROW(D15)-1,0)),F15)</f>
-        <v>Respuesta Corta</v>
+        <v>Short Answer</v>
       </c>
       <c r="F15" s="148" t="s">
         <v>8</v>
@@ -24161,11 +24173,11 @@
       </c>
       <c r="T15" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U15" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Palabra Perdida </v>
+        <v xml:space="preserve">Missing Word </v>
       </c>
       <c r="V15" s="191" t="s">
         <v>574</v>
@@ -24198,7 +24210,7 @@
       </c>
       <c r="AE15" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF15" s="179"/>
     </row>
@@ -24217,7 +24229,7 @@
       <c r="D16" s="169"/>
       <c r="E16" s="147" t="str">
         <f>IFERROR(IF(D16&lt;&gt;"",D16,HLOOKUP($E$2,$F$2:K16,ROW(D16)-1,0)),F16)</f>
-        <v>Palabra Perdida</v>
+        <v>Missing Word</v>
       </c>
       <c r="F16" s="147" t="s">
         <v>9</v>
@@ -24262,11 +24274,11 @@
       </c>
       <c r="T16" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U16" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">Ensayo </v>
+        <v xml:space="preserve">Essay </v>
       </c>
       <c r="V16" s="191" t="s">
         <v>575</v>
@@ -24299,7 +24311,7 @@
       </c>
       <c r="AE16" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF16" s="179"/>
     </row>
@@ -24363,7 +24375,7 @@
       </c>
       <c r="T17" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="U17" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
@@ -24400,7 +24412,7 @@
       </c>
       <c r="AE17" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="AF17" s="179"/>
     </row>
@@ -24419,7 +24431,7 @@
       <c r="D18" s="169"/>
       <c r="E18" s="147" t="str">
         <f>IFERROR(IF(D18&lt;&gt;"",D18,HLOOKUP($E$2,$F$2:K18,ROW(D18)-1,0)),F18)</f>
-        <v>Preguntas</v>
+        <v>Questions</v>
       </c>
       <c r="F18" s="147" t="s">
         <v>6</v>
@@ -24464,11 +24476,11 @@
       </c>
       <c r="T18" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 1]]&amp;IDIOMA),"")</f>
-        <v>LINK DICCIONARIO</v>
+        <v>LINK DICTIONARY</v>
       </c>
       <c r="U18" s="191" t="str">
         <f ca="1">IFERROR(INDIRECT(Tabla_Menu[[#This Row],[Nivel 2]]&amp;IDIOMA)&amp;IF(Tabla_Menu[[#This Row],[Nivel]]="",""," "&amp;Tabla_Menu[[#This Row],['[Teclas']]]),"")</f>
-        <v xml:space="preserve">LINK DICCIONARIO </v>
+        <v xml:space="preserve">LINK DICTIONARY </v>
       </c>
       <c r="V18" s="191" t="s">
         <v>577</v>
@@ -24501,7 +24513,7 @@
       </c>
       <c r="AE18" s="181" t="str">
         <f ca="1">Tabla_Menu[[#This Row],[Nivel]]&amp;Tabla_Menu[[#This Row],[N/A]]</f>
-        <v>LINK DICCIONARIO</v>
+        <v>LINK DICTIONARY</v>
       </c>
       <c r="AF18" s="179"/>
     </row>
@@ -24520,7 +24532,7 @@
       <c r="D19" s="170"/>
       <c r="E19" s="148" t="str">
         <f>IFERROR(IF(D19&lt;&gt;"",D19,HLOOKUP($E$2,$F$2:K19,ROW(D19)-1,0)),F19)</f>
-        <v>Ensayo</v>
+        <v>Essay</v>
       </c>
       <c r="F19" s="148" t="s">
         <v>206</v>
@@ -24611,7 +24623,7 @@
       <c r="D20" s="169"/>
       <c r="E20" s="147" t="str">
         <f>IFERROR(IF(D20&lt;&gt;"",D20,HLOOKUP($E$2,$F$2:K20,ROW(D20)-1,0)),F20)</f>
-        <v>PERSONALIZAR DICCIONARIO</v>
+        <v>CUSTOM DICTIONARY</v>
       </c>
       <c r="F20" s="147" t="s">
         <v>393</v>
@@ -24697,7 +24709,7 @@
       <c r="D21" s="168"/>
       <c r="E21" s="146" t="str">
         <f>IFERROR(IF(D21&lt;&gt;"",D21,HLOOKUP($E$2,$F$2:K21,ROW(D21)-1,0)),F21)</f>
-        <v>Banco de preguntas</v>
+        <v>Question database</v>
       </c>
       <c r="F21" s="146" t="s">
         <v>87</v>
@@ -24788,7 +24800,7 @@
       <c r="D22" s="169"/>
       <c r="E22" s="147" t="str">
         <f>IFERROR(IF(D22&lt;&gt;"",D22,HLOOKUP($E$2,$F$2:K22,ROW(D22)-1,0)),F22)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="F22" s="147" t="s">
         <v>93</v>
@@ -24879,7 +24891,7 @@
       <c r="D23" s="170"/>
       <c r="E23" s="148" t="str">
         <f>IFERROR(IF(D23&lt;&gt;"",D23,HLOOKUP($E$2,$F$2:K23,ROW(D23)-1,0)),F23)</f>
-        <v>DICCIONARIO</v>
+        <v>DICTIONARY</v>
       </c>
       <c r="F23" s="148" t="s">
         <v>391</v>
@@ -24963,7 +24975,7 @@
       <c r="D24" s="169"/>
       <c r="E24" s="147" t="str">
         <f>IFERROR(IF(D24&lt;&gt;"",D24,HLOOKUP($E$2,$F$2:K24,ROW(D24)-1,0)),F24)</f>
-        <v>Enunciado de la pregunta</v>
+        <v>Question statement</v>
       </c>
       <c r="F24" s="147" t="s">
         <v>99</v>
@@ -25047,7 +25059,7 @@
       <c r="D25" s="170"/>
       <c r="E25" s="148" t="str">
         <f>IFERROR(IF(D25&lt;&gt;"",D25,HLOOKUP($E$2,$F$2:K25,ROW(D25)-1,0)),F25)</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F25" s="148" t="s">
         <v>105</v>
@@ -25131,7 +25143,7 @@
       <c r="D26" s="169"/>
       <c r="E26" s="147" t="str">
         <f>IFERROR(IF(D26&lt;&gt;"",D26,HLOOKUP($E$2,$F$2:K26,ROW(D26)-1,0)),F26)</f>
-        <v>Respuesta Correcta</v>
+        <v>Right Answer</v>
       </c>
       <c r="F26" s="147" t="s">
         <v>110</v>
@@ -25215,7 +25227,7 @@
       <c r="D27" s="170"/>
       <c r="E27" s="148" t="str">
         <f>IFERROR(IF(D27&lt;&gt;"",D27,HLOOKUP($E$2,$F$2:K27,ROW(D27)-1,0)),F27)</f>
-        <v>Respuesta Incorrecta</v>
+        <v>Wrong Answer</v>
       </c>
       <c r="F27" s="148" t="s">
         <v>116</v>
@@ -25299,7 +25311,7 @@
       <c r="D28" s="169"/>
       <c r="E28" s="147" t="str">
         <f>IFERROR(IF(D28&lt;&gt;"",D28,HLOOKUP($E$2,$F$2:K28,ROW(D28)-1,0)),F28)</f>
-        <v>Retroalim.</v>
+        <v>Feedback</v>
       </c>
       <c r="F28" s="147" t="s">
         <v>122</v>
@@ -25383,7 +25395,7 @@
       <c r="D29" s="170"/>
       <c r="E29" s="148" t="str">
         <f>IFERROR(IF(D29&lt;&gt;"",D29,HLOOKUP($E$2,$F$2:K29,ROW(D29)-1,0)),F29)</f>
-        <v>Pista</v>
+        <v>Hint</v>
       </c>
       <c r="F29" s="148" t="s">
         <v>127</v>
@@ -25467,7 +25479,7 @@
       <c r="D30" s="169"/>
       <c r="E30" s="147" t="str">
         <f>IFERROR(IF(D30&lt;&gt;"",D30,HLOOKUP($E$2,$F$2:K30,ROW(D30)-1,0)),F30)</f>
-        <v>Puntos</v>
+        <v>Points</v>
       </c>
       <c r="F30" s="147" t="s">
         <v>133</v>
@@ -25532,7 +25544,7 @@
       <c r="D31" s="170"/>
       <c r="E31" s="148" t="str">
         <f>IFERROR(IF(D31&lt;&gt;"",D31,HLOOKUP($E$2,$F$2:K31,ROW(D31)-1,0)),F31)</f>
-        <v>OM 1R</v>
+        <v>MC 1A</v>
       </c>
       <c r="F31" s="148" t="s">
         <v>138</v>
@@ -25583,7 +25595,7 @@
       <c r="D32" s="169"/>
       <c r="E32" s="147" t="str">
         <f>IFERROR(IF(D32&lt;&gt;"",D32,HLOOKUP($E$2,$F$2:K32,ROW(D32)-1,0)),F32)</f>
-        <v>OM +R</v>
+        <v>MC +A</v>
       </c>
       <c r="F32" s="147" t="s">
         <v>478</v>
@@ -25634,7 +25646,7 @@
       <c r="D33" s="170"/>
       <c r="E33" s="148" t="str">
         <f>IFERROR(IF(D33&lt;&gt;"",D33,HLOOKUP($E$2,$F$2:K33,ROW(D33)-1,0)),F33)</f>
-        <v>VF</v>
+        <v>TF</v>
       </c>
       <c r="F33" s="148" t="s">
         <v>143</v>
@@ -25685,7 +25697,7 @@
       <c r="D34" s="169"/>
       <c r="E34" s="147" t="str">
         <f>IFERROR(IF(D34&lt;&gt;"",D34,HLOOKUP($E$2,$F$2:K34,ROW(D34)-1,0)),F34)</f>
-        <v>EM</v>
+        <v>MA</v>
       </c>
       <c r="F34" s="147" t="s">
         <v>146</v>
@@ -25736,7 +25748,7 @@
       <c r="D35" s="170"/>
       <c r="E35" s="148" t="str">
         <f>IFERROR(IF(D35&lt;&gt;"",D35,HLOOKUP($E$2,$F$2:K35,ROW(D35)-1,0)),F35)</f>
-        <v>RC</v>
+        <v>SA</v>
       </c>
       <c r="F35" s="148" t="s">
         <v>151</v>
@@ -25787,7 +25799,7 @@
       <c r="D36" s="169"/>
       <c r="E36" s="147" t="str">
         <f>IFERROR(IF(D36&lt;&gt;"",D36,HLOOKUP($E$2,$F$2:K36,ROW(D36)-1,0)),F36)</f>
-        <v>PP</v>
+        <v>MW</v>
       </c>
       <c r="F36" s="147" t="s">
         <v>155</v>
@@ -25898,7 +25910,7 @@
       <c r="D38" s="169"/>
       <c r="E38" s="147" t="str">
         <f>IFERROR(IF(D38&lt;&gt;"",D38,HLOOKUP($E$2,$F$2:K38,ROW(D38)-1,0)),F38)</f>
-        <v xml:space="preserve">Pareja </v>
+        <v xml:space="preserve">Pair </v>
       </c>
       <c r="F38" s="147" t="s">
         <v>162</v>
@@ -25958,7 +25970,7 @@
       <c r="D39" s="170"/>
       <c r="E39" s="148" t="str">
         <f>IFERROR(IF(D39&lt;&gt;"",D39,HLOOKUP($E$2,$F$2:K39,ROW(D39)-1,0)),F39)</f>
-        <v>Mayúsculas</v>
+        <v>Capitalization</v>
       </c>
       <c r="F39" s="148" t="s">
         <v>3</v>
@@ -26018,7 +26030,7 @@
       <c r="D40" s="169"/>
       <c r="E40" s="147" t="str">
         <f>IFERROR(IF(D40&lt;&gt;"",D40,HLOOKUP($E$2,$F$2:K40,ROW(D40)-1,0)),F40)</f>
-        <v>Respuesta</v>
+        <v>Answer</v>
       </c>
       <c r="F40" s="147" t="s">
         <v>175</v>
@@ -26078,7 +26090,7 @@
       <c r="D41" s="170"/>
       <c r="E41" s="148" t="str">
         <f>IFERROR(IF(D41&lt;&gt;"",D41,HLOOKUP($E$2,$F$2:K41,ROW(D41)-1,0)),F41)</f>
-        <v xml:space="preserve">Palabra </v>
+        <v xml:space="preserve">Word </v>
       </c>
       <c r="F41" s="148" t="s">
         <v>181</v>
@@ -26138,7 +26150,7 @@
       <c r="D42" s="169"/>
       <c r="E42" s="147" t="str">
         <f>IFERROR(IF(D42&lt;&gt;"",D42,HLOOKUP($E$2,$F$2:K42,ROW(D42)-1,0)),F42)</f>
-        <v>VERDADERO</v>
+        <v>TRUE</v>
       </c>
       <c r="F42" s="147" t="s">
         <v>188</v>
@@ -26198,7 +26210,7 @@
       <c r="D43" s="170"/>
       <c r="E43" s="148" t="str">
         <f>IFERROR(IF(D43&lt;&gt;"",D43,HLOOKUP($E$2,$F$2:K43,ROW(D43)-1,0)),F43)</f>
-        <v>FALSO</v>
+        <v>FALSE</v>
       </c>
       <c r="F43" s="148" t="s">
         <v>195</v>
@@ -26258,7 +26270,7 @@
       <c r="D44" s="169"/>
       <c r="E44" s="147" t="str">
         <f>IFERROR(IF(D44&lt;&gt;"",D44,HLOOKUP($E$2,$F$2:K44,ROW(D44)-1,0)),F44)</f>
-        <v xml:space="preserve">Grupo </v>
+        <v xml:space="preserve">Group </v>
       </c>
       <c r="F44" s="147" t="s">
         <v>200</v>
@@ -26321,7 +26333,7 @@
       <c r="D45" s="170"/>
       <c r="E45" s="148" t="str">
         <f>IFERROR(IF(D45&lt;&gt;"",D45,HLOOKUP($E$2,$F$2:K45,ROW(D45)-1,0)),F45)</f>
-        <v>Formato de la Respuesta</v>
+        <v>Response format</v>
       </c>
       <c r="F45" s="148" t="s">
         <v>212</v>
@@ -26372,7 +26384,7 @@
       <c r="D46" s="169"/>
       <c r="E46" s="147" t="str">
         <f>IFERROR(IF(D46&lt;&gt;"",D46,HLOOKUP($E$2,$F$2:K46,ROW(D46)-1,0)),F46)</f>
-        <v>Requerir texto</v>
+        <v>Require text</v>
       </c>
       <c r="F46" s="147" t="s">
         <v>218</v>
@@ -26423,7 +26435,7 @@
       <c r="D47" s="170"/>
       <c r="E47" s="148" t="str">
         <f>IFERROR(IF(D47&lt;&gt;"",D47,HLOOKUP($E$2,$F$2:K47,ROW(D47)-1,0)),F47)</f>
-        <v>Tamaño de la caja de entrada</v>
+        <v>Input box size</v>
       </c>
       <c r="F47" s="148" t="s">
         <v>224</v>
@@ -26471,7 +26483,7 @@
       <c r="D48" s="169"/>
       <c r="E48" s="147" t="str">
         <f>IFERROR(IF(D48&lt;&gt;"",D48,HLOOKUP($E$2,$F$2:K48,ROW(D48)-1,0)),F48)</f>
-        <v>Permitir archivos adjuntos</v>
+        <v>Allow attachments</v>
       </c>
       <c r="F48" s="147" t="s">
         <v>230</v>
@@ -26519,7 +26531,7 @@
       <c r="D49" s="170"/>
       <c r="E49" s="148" t="str">
         <f>IFERROR(IF(D49&lt;&gt;"",D49,HLOOKUP($E$2,$F$2:K49,ROW(D49)-1,0)),F49)</f>
-        <v>Archivos adjuntos requeridos</v>
+        <v>Require attachments</v>
       </c>
       <c r="F49" s="148" t="s">
         <v>236</v>
@@ -26567,7 +26579,7 @@
       <c r="D50" s="169"/>
       <c r="E50" s="147" t="str">
         <f>IFERROR(IF(D50&lt;&gt;"",D50,HLOOKUP($E$2,$F$2:K50,ROW(D50)-1,0)),F50)</f>
-        <v>Plantilla de Respuesta</v>
+        <v>Response template</v>
       </c>
       <c r="F50" s="147" t="s">
         <v>242</v>
@@ -26615,7 +26627,7 @@
       <c r="D51" s="170"/>
       <c r="E51" s="148" t="str">
         <f>IFERROR(IF(D51&lt;&gt;"",D51,HLOOKUP($E$2,$F$2:K51,ROW(D51)-1,0)),F51)</f>
-        <v>Información para el evaluador</v>
+        <v>Information for graders</v>
       </c>
       <c r="F51" s="148" t="s">
         <v>248</v>
@@ -26657,7 +26669,7 @@
       <c r="D52" s="169"/>
       <c r="E52" s="147" t="str">
         <f>IFERROR(IF(D52&lt;&gt;"",D52,HLOOKUP($E$2,$F$2:K52,ROW(D52)-1,0)),F52)</f>
-        <v>EN</v>
+        <v>ES</v>
       </c>
       <c r="F52" s="147" t="s">
         <v>211</v>
@@ -26699,7 +26711,7 @@
       <c r="D53" s="170"/>
       <c r="E53" s="148" t="str">
         <f>IFERROR(IF(D53&lt;&gt;"",D53,HLOOKUP($E$2,$F$2:K53,ROW(D53)-1,0)),F53)</f>
-        <v>Ancho RC</v>
+        <v>Width SA</v>
       </c>
       <c r="F53" s="148" t="s">
         <v>269</v>
@@ -26741,7 +26753,7 @@
       <c r="D54" s="169"/>
       <c r="E54" s="147" t="str">
         <f>IFERROR(IF(D54&lt;&gt;"",D54,HLOOKUP($E$2,$F$2:K54,ROW(D54)-1,0)),F54)</f>
-        <v>Nº max. Respuestas</v>
+        <v>No. max. Answers</v>
       </c>
       <c r="F54" s="147" t="s">
         <v>718</v>
@@ -26782,7 +26794,7 @@
       <c r="D55" s="168"/>
       <c r="E55" s="146" t="str">
         <f>IFERROR(IF(D55&lt;&gt;"",D55,HLOOKUP($E$2,$F$2:K55,ROW(D55)-1,0)),F55)</f>
-        <v>MENSAJES MACROS</v>
+        <v>MACROS MESSAGES</v>
       </c>
       <c r="F55" s="146" t="s">
         <v>439</v>
@@ -26830,8 +26842,8 @@
       <c r="D56" s="169"/>
       <c r="E56" s="147" t="str">
         <f>IFERROR(IF(D56&lt;&gt;"",D56,HLOOKUP($E$2,$F$2:K56,ROW(D56)-1,0)),F56)</f>
-        <v>Copia el link (Ctrl+C) y 
-pega (Ctrl+V) en Internet.</v>
+        <v>Copy the link (Ctrl + C), 
+and paste (Ctrl + V) in Internet.</v>
       </c>
       <c r="F56" s="147" t="s">
         <v>442</v>
@@ -26870,7 +26882,7 @@
       <c r="D57" s="170"/>
       <c r="E57" s="148" t="str">
         <f>IFERROR(IF(D57&lt;&gt;"",D57,HLOOKUP($E$2,$F$2:K57,ROW(D57)-1,0)),F57)</f>
-        <v>MENÚ GENERAL</v>
+        <v>GENERAL MENU</v>
       </c>
       <c r="F57" s="148" t="s">
         <v>507</v>
@@ -26909,7 +26921,7 @@
       <c r="D58" s="169"/>
       <c r="E58" s="147" t="str">
         <f>IFERROR(IF(D58&lt;&gt;"",D58,HLOOKUP($E$2,$F$2:K58,ROW(D58)-1,0)),F58)</f>
-        <v xml:space="preserve">GUARDAR </v>
+        <v>SAVE</v>
       </c>
       <c r="F58" s="147" t="s">
         <v>514</v>
@@ -26948,7 +26960,7 @@
       <c r="D59" s="170"/>
       <c r="E59" s="148" t="str">
         <f>IFERROR(IF(D59&lt;&gt;"",D59,HLOOKUP($E$2,$F$2:K59,ROW(D59)-1,0)),F59)</f>
-        <v>CERRAR</v>
+        <v>CLOSE</v>
       </c>
       <c r="F59" s="148" t="s">
         <v>521</v>
@@ -26987,7 +26999,7 @@
       <c r="D60" s="169"/>
       <c r="E60" s="147" t="str">
         <f>IFERROR(IF(D60&lt;&gt;"",D60,HLOOKUP($E$2,$F$2:K60,ROW(D60)-1,0)),F60)</f>
-        <v>AYUDA</v>
+        <v>HELP</v>
       </c>
       <c r="F60" s="147" t="s">
         <v>528</v>
@@ -27026,7 +27038,7 @@
       <c r="D61" s="170"/>
       <c r="E61" s="148" t="str">
         <f>IFERROR(IF(D61&lt;&gt;"",D61,HLOOKUP($E$2,$F$2:K61,ROW(D61)-1,0)),F61)</f>
-        <v>COPIAR</v>
+        <v>COPY</v>
       </c>
       <c r="F61" s="148" t="s">
         <v>535</v>
@@ -27065,7 +27077,7 @@
       <c r="D62" s="169"/>
       <c r="E62" s="147" t="str">
         <f>IFERROR(IF(D62&lt;&gt;"",D62,HLOOKUP($E$2,$F$2:K62,ROW(D62)-1,0)),F62)</f>
-        <v>PEGAR</v>
+        <v>PASTE</v>
       </c>
       <c r="F62" s="147" t="s">
         <v>542</v>
@@ -27104,7 +27116,7 @@
       <c r="D63" s="170"/>
       <c r="E63" s="148" t="str">
         <f>IFERROR(IF(D63&lt;&gt;"",D63,HLOOKUP($E$2,$F$2:K63,ROW(D63)-1,0)),F63)</f>
-        <v>IR A…</v>
+        <v>GO TO …</v>
       </c>
       <c r="F63" s="148" t="s">
         <v>549</v>
@@ -27143,7 +27155,7 @@
       <c r="D64" s="169"/>
       <c r="E64" s="147" t="str">
         <f>IFERROR(IF(D64&lt;&gt;"",D64,HLOOKUP($E$2,$F$2:K64,ROW(D64)-1,0)),F64)</f>
-        <v>LINK DICCIONARIO</v>
+        <v>LINK DICTIONARY</v>
       </c>
       <c r="F64" s="147" t="s">
         <v>557</v>
@@ -27182,7 +27194,7 @@
       <c r="D65" s="170"/>
       <c r="E65" s="148" t="str">
         <f>IFERROR(IF(D65&lt;&gt;"",D65,HLOOKUP($E$2,$F$2:K65,ROW(D65)-1,0)),F65)</f>
-        <v>MENU EXCEL</v>
+        <v>EXCEL MENU</v>
       </c>
       <c r="F65" s="148" t="s">
         <v>645</v>
@@ -27221,7 +27233,7 @@
       <c r="D66" s="169"/>
       <c r="E66" s="147" t="str">
         <f>IFERROR(IF(D66&lt;&gt;"",D66,HLOOKUP($E$2,$F$2:K66,ROW(D66)-1,0)),F66)</f>
-        <v>¿Desea guardar los cambios?</v>
+        <v>Do you want to save your changes?</v>
       </c>
       <c r="F66" s="147" t="s">
         <v>653</v>
@@ -27260,7 +27272,7 @@
       <c r="D67" s="195"/>
       <c r="E67" s="195" t="str">
         <f>IFERROR(IF(D67&lt;&gt;"",D67,HLOOKUP($E$2,$F$2:K67,ROW(D67)-1,0)),F67)</f>
-        <v>FIN</v>
+        <v>END</v>
       </c>
       <c r="F67" s="195" t="s">
         <v>725</v>
@@ -27797,13 +27809,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="EFvDi3MSRW73NdIsYvAsc+BhgNAxKxcPxTt3ACKCjR73QNbhqIfRpAgCELXZUjGGqLKgcIubArfstFoT9O9iow==" saltValue="M4mqjZOIoId7mfBIEVvyPQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="F3:F53 F55">
-    <cfRule type="duplicateValues" dxfId="43" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="duplicateValues" dxfId="42" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:F66">
-    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W38:W43 X3:X29" xr:uid="{00000000-0002-0000-0900-000000000000}">
@@ -27832,10 +27844,10 @@
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5:AI7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -27856,11 +27868,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">INDIRECT("Z_BP_10_"&amp;IDIOMA)&amp;"                  "&amp;INDIRECT("Z_BP_11_"&amp;IDIOMA)&amp;"                    "&amp;INDIRECT("Z_BP_12_"&amp;IDIOMA)&amp;"                         "&amp;INDIRECT("Z_BP_13_"&amp;IDIOMA)&amp;"                                "&amp;INDIRECT("Z_IN_00_"&amp;IDIOMA)</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="H1" s="183"/>
       <c r="J1" s="35"/>
@@ -27894,7 +27906,7 @@
       <c r="E2"/>
       <c r="F2" s="60" t="str">
         <f ca="1">"    "&amp;INDIRECT("Z_BP_14_"&amp;IDIOMA)&amp;"                         "&amp;INDIRECT("Z_BP_15_"&amp;IDIOMA)&amp;"                         "&amp;INDIRECT("Z_BP_31_"&amp;IDIOMA)&amp;"                         "&amp;INDIRECT("Z_BP_16_"&amp;IDIOMA)&amp;"                                 "&amp;INDIRECT("Z_BP_02_"&amp;IDIOMA)</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_OM[Enunciado])</f>
@@ -27904,95 +27916,95 @@
     <row r="3" spans="1:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="52" t="str">
         <f ca="1">"N. "&amp;INDIRECT("Z_BP_05_"&amp;IDIOMA)</f>
-        <v>N. Respuesta Correcta</v>
+        <v>N. Right Answer</v>
       </c>
       <c r="B3" s="52" t="str">
         <f ca="1">"N. "&amp;INDIRECT("Z_BP_06_"&amp;IDIOMA)</f>
-        <v>N. Respuesta Incorrecta</v>
+        <v>N. Wrong Answer</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22" t="str">
         <f ca="1">INDIRECT("Z_BP_04_"&amp;IDIOMA)</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!C24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - OPCIÓN MÚLTIPLE 1R 
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - MULTIPLE CHOICE 1A
+Question statement</v>
       </c>
       <c r="G3" s="67" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Respuesta 1</v>
+        <v>Answer 1</v>
       </c>
       <c r="H3" s="68" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Respuesta 2</v>
+        <v>Answer 2</v>
       </c>
       <c r="I3" s="69" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Respuesta 3</v>
+        <v>Answer 3</v>
       </c>
       <c r="J3" s="70" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Respuesta 4</v>
+        <v>Answer 4</v>
       </c>
       <c r="K3" s="71" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 5"</f>
-        <v>Respuesta 5</v>
+        <v>Answer 5</v>
       </c>
       <c r="L3" s="72" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 6"</f>
-        <v>Respuesta 6</v>
+        <v>Answer 6</v>
       </c>
       <c r="M3" s="73" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Retroalim. 1</v>
+        <v>Feedback 1</v>
       </c>
       <c r="N3" s="74" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Retroalim. 2</v>
+        <v>Feedback 2</v>
       </c>
       <c r="O3" s="75" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Retroalim. 3</v>
+        <v>Feedback 3</v>
       </c>
       <c r="P3" s="79" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Retroalim. 4</v>
+        <v>Feedback 4</v>
       </c>
       <c r="Q3" s="80" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 5"</f>
-        <v>Retroalim. 5</v>
+        <v>Feedback 5</v>
       </c>
       <c r="R3" s="81" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 6"</f>
-        <v>Retroalim. 6</v>
+        <v>Feedback 6</v>
       </c>
       <c r="S3" s="73" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Puntos 1</v>
+        <v>Points 1</v>
       </c>
       <c r="T3" s="74" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Puntos 2</v>
+        <v>Points 2</v>
       </c>
       <c r="U3" s="75" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Puntos 3</v>
+        <v>Points 3</v>
       </c>
       <c r="V3" s="79" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Puntos 4</v>
+        <v>Points 4</v>
       </c>
       <c r="W3" s="80" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 5"</f>
-        <v>Puntos 5</v>
+        <v>Points 5</v>
       </c>
       <c r="X3" s="81" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 6"</f>
-        <v>Puntos 6</v>
+        <v>Points 6</v>
       </c>
       <c r="Y3" s="81"/>
       <c r="Z3" s="81"/>
@@ -28002,19 +28014,19 @@
       <c r="AD3" s="81"/>
       <c r="AE3" s="82" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="83" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="84" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="85" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="s">
         <v>279</v>
@@ -28342,7 +28354,7 @@
       <c r="AI7" s="86"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="iNgiwAgmThDRYPx9RdtkSArnFP7eW/MBCJtjxNn6203T1mylASS2R/vBtvrMBi+PHw2I30wwM6f7OkCRpVXlTQ==" saltValue="oTlWlfZlMWT4yXhYDbBvMw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xDcBKiWKRHDy790EfY8tPTtXY2L/w+ozYjrWULIVz+T77i4369VCsNiGbyuUkHHjV+aVfemvGIVUsatGr6Njfg==" saltValue="Lae1QVfoiAnYdbocf3yiEg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -28364,7 +28376,7 @@
       <selection pane="bottomRight" activeCell="E5" sqref="E5:AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -28386,11 +28398,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -28423,7 +28435,7 @@
       <c r="E2"/>
       <c r="F2" s="59" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_O2[Enunciado])</f>
@@ -28433,99 +28445,99 @@
     <row r="3" spans="1:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="52" t="str">
         <f ca="1">"N. "&amp;INDIRECT("Z_BP_05_"&amp;IDIOMA)</f>
-        <v>N. Respuesta Correcta</v>
+        <v>N. Right Answer</v>
       </c>
       <c r="B3" s="52" t="str">
         <f ca="1">"N. "&amp;INDIRECT("Z_BP_06_"&amp;IDIOMA)</f>
-        <v>N. Respuesta Incorrecta</v>
+        <v>N. Wrong Answer</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22" t="str">
         <f ca="1">INDIRECT("Z_BP_04_"&amp;IDIOMA)</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!E24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - OPCIÓN MÚLTIPLE +R 
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - MULTIPLE CHOICE +A
+Question statement</v>
       </c>
       <c r="G3" s="67" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Respuesta 1</v>
+        <v>Answer 1</v>
       </c>
       <c r="H3" s="68" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Respuesta 2</v>
+        <v>Answer 2</v>
       </c>
       <c r="I3" s="69" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Respuesta 3</v>
+        <v>Answer 3</v>
       </c>
       <c r="J3" s="70" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Respuesta 4</v>
+        <v>Answer 4</v>
       </c>
       <c r="K3" s="71" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 5"</f>
-        <v>Respuesta 5</v>
+        <v>Answer 5</v>
       </c>
       <c r="L3" s="72" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)&amp;" 6"</f>
-        <v>Respuesta 6</v>
+        <v>Answer 6</v>
       </c>
       <c r="M3" s="73" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Retroalim. 1</v>
+        <v>Feedback 1</v>
       </c>
       <c r="N3" s="74" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Retroalim. 2</v>
+        <v>Feedback 2</v>
       </c>
       <c r="O3" s="75" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Retroalim. 3</v>
+        <v>Feedback 3</v>
       </c>
       <c r="P3" s="79" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Retroalim. 4</v>
+        <v>Feedback 4</v>
       </c>
       <c r="Q3" s="80" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 5"</f>
-        <v>Retroalim. 5</v>
+        <v>Feedback 5</v>
       </c>
       <c r="R3" s="81" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 6"</f>
-        <v>Retroalim. 6</v>
+        <v>Feedback 6</v>
       </c>
       <c r="S3" s="73" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Puntos 1</v>
+        <v>Points 1</v>
       </c>
       <c r="T3" s="74" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Puntos 2</v>
+        <v>Points 2</v>
       </c>
       <c r="U3" s="75" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Puntos 3</v>
+        <v>Points 3</v>
       </c>
       <c r="V3" s="79" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Puntos 4</v>
+        <v>Points 4</v>
       </c>
       <c r="W3" s="80" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 5"</f>
-        <v>Puntos 5</v>
+        <v>Points 5</v>
       </c>
       <c r="X3" s="81" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 6"</f>
-        <v>Puntos 6</v>
+        <v>Points 6</v>
       </c>
       <c r="Y3" s="200" t="str">
         <f ca="1">INDIRECT("Z_BP_33_"&amp; IDIOMA)</f>
-        <v>Nº max. Respuestas</v>
+        <v>No. max. Answers</v>
       </c>
       <c r="Z3" s="81"/>
       <c r="AA3" s="81"/>
@@ -28534,19 +28546,19 @@
       <c r="AD3" s="81"/>
       <c r="AE3" s="82" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 1"</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="83" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 2"</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="84" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 3"</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="85" t="str">
         <f ca="1">INDIRECT("Z_BP_08_"&amp;IDIOMA)&amp;" 4"</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="str">
         <f>'Datos OM'!AI3</f>
@@ -28809,7 +28821,7 @@
       <c r="AI6" s="86"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5fhxDoHngt5bItu/nN+XLVnC0paVK5SArHe6Ya5cs07PaJNCmEkaqyZvd2RQ5bZ3xks2aB0QTjWdJMcj8WGDww==" saltValue="l9bOvB2MHhdEcgg3pvlH/g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XHioHYO4w7H6D4UjkloIl3toVVji9q96EtgNmMpMhcH2pjwuZokb8tLhLj+MxQ80EwyAeJVZ4fORD2w+H5MsKQ==" saltValue="vDCuAoKFjmQOg1TcvmlUng==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -28830,7 +28842,7 @@
       <selection pane="bottomRight" activeCell="E5" sqref="E5:AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -28851,11 +28863,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -28888,7 +28900,7 @@
       <c r="E2"/>
       <c r="F2" s="59" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_VF[Enunciado])</f>
@@ -28902,25 +28914,25 @@
       <c r="D3" s="21"/>
       <c r="E3" s="22" t="str">
         <f ca="1">INDIRECT("Z_BP_04_"&amp;IDIOMA)</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!G24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - VERDADERO/FALSO
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - TRUE/FALSE
+Question statement</v>
       </c>
       <c r="G3" s="67" t="str">
         <f ca="1">'Datos OM'!G3</f>
-        <v>Respuesta 1</v>
+        <v>Answer 1</v>
       </c>
       <c r="H3" s="74" t="str">
         <f ca="1">'Datos OM'!M3</f>
-        <v>Retroalim. 1</v>
+        <v>Feedback 1</v>
       </c>
       <c r="I3" s="75" t="str">
         <f ca="1">'Datos OM'!N3</f>
-        <v>Retroalim. 2</v>
+        <v>Feedback 2</v>
       </c>
       <c r="J3" s="79"/>
       <c r="K3" s="80"/>
@@ -28945,19 +28957,19 @@
       <c r="AD3" s="81"/>
       <c r="AE3" s="82" t="str">
         <f ca="1">'Datos OM'!AE3</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="83" t="str">
         <f ca="1">'Datos OM'!AF3</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="84" t="str">
         <f ca="1">'Datos OM'!AG3</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="85" t="str">
         <f ca="1">'Datos OM'!AH3</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="str">
         <f>'Datos OM'!AI3</f>
@@ -29186,7 +29198,7 @@
       <c r="AI6" s="66"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KY7nH4z5oZNn6gpGfNJBv0SFcv7mFR+qq8egz5QLTIxZ80iqAaXKrRtZqJw2YRAe44nC8qKi5x6E/1RhSSwjnw==" saltValue="qRQMnAo8WxMrhZ5kNP8lyQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="s5ZPL8x9zBAAIcBfCOxSj5ZAyYufEuLzZlw2dZjHNQ8vzMN6thV7Hd+k26Eq/H/MRzXHPOTLFELuoemh6py/zw==" saltValue="OCqzJuFIGjhuEtS9B02aLQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -29207,7 +29219,7 @@
       <selection pane="bottomRight" activeCell="E5" sqref="E5:AI7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -29229,11 +29241,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -29266,7 +29278,7 @@
       <c r="E2"/>
       <c r="F2" s="59" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_EM[Enunciado])</f>
@@ -29276,132 +29288,132 @@
     <row r="3" spans="1:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="61" t="str">
         <f ca="1">INDIRECT("Z_BP_17_"&amp;IDIOMA)</f>
-        <v xml:space="preserve">Pareja </v>
+        <v xml:space="preserve">Pair </v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="22" t="str">
         <f ca="1">'Datos OM'!E3</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!I24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - EMPAREJAR
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - MATCHING
+Question statement</v>
       </c>
       <c r="G3" s="103" t="str">
         <f ca="1">$A$3&amp;" 01.1"</f>
-        <v>Pareja  01.1</v>
+        <v>Pair  01.1</v>
       </c>
       <c r="H3" s="103" t="str">
         <f ca="1">$A$3&amp;" 01.2"</f>
-        <v>Pareja  01.2</v>
+        <v>Pair  01.2</v>
       </c>
       <c r="I3" s="105" t="str">
         <f ca="1">$A$3&amp;" 02.1"</f>
-        <v>Pareja  02.1</v>
+        <v>Pair  02.1</v>
       </c>
       <c r="J3" s="105" t="str">
         <f ca="1">$A$3&amp;" 02.2"</f>
-        <v>Pareja  02.2</v>
+        <v>Pair  02.2</v>
       </c>
       <c r="K3" s="132" t="str">
         <f ca="1">$A$3&amp;" 03.1"</f>
-        <v>Pareja  03.1</v>
+        <v>Pair  03.1</v>
       </c>
       <c r="L3" s="132" t="str">
         <f ca="1">$A$3&amp;" 03.2"</f>
-        <v>Pareja  03.2</v>
+        <v>Pair  03.2</v>
       </c>
       <c r="M3" s="107" t="str">
         <f ca="1">$A$3&amp;" 04.1"</f>
-        <v>Pareja  04.1</v>
+        <v>Pair  04.1</v>
       </c>
       <c r="N3" s="107" t="str">
         <f ca="1">$A$3&amp;" 04.2"</f>
-        <v>Pareja  04.2</v>
+        <v>Pair  04.2</v>
       </c>
       <c r="O3" s="109" t="str">
         <f ca="1">$A$3&amp;" 05.1"</f>
-        <v>Pareja  05.1</v>
+        <v>Pair  05.1</v>
       </c>
       <c r="P3" s="109" t="str">
         <f ca="1">$A$3&amp;" 05.2"</f>
-        <v>Pareja  05.2</v>
+        <v>Pair  05.2</v>
       </c>
       <c r="Q3" s="111" t="str">
         <f ca="1">$A$3&amp;" 06.1"</f>
-        <v>Pareja  06.1</v>
+        <v>Pair  06.1</v>
       </c>
       <c r="R3" s="111" t="str">
         <f ca="1">$A$3&amp;" 06.2"</f>
-        <v>Pareja  06.2</v>
+        <v>Pair  06.2</v>
       </c>
       <c r="S3" s="103" t="str">
         <f ca="1">$A$3&amp;" 07.1"</f>
-        <v>Pareja  07.1</v>
+        <v>Pair  07.1</v>
       </c>
       <c r="T3" s="103" t="str">
         <f ca="1">$A$3&amp;" 07.2"</f>
-        <v>Pareja  07.2</v>
+        <v>Pair  07.2</v>
       </c>
       <c r="U3" s="105" t="str">
         <f ca="1">$A$3&amp;" 08.1"</f>
-        <v>Pareja  08.1</v>
+        <v>Pair  08.1</v>
       </c>
       <c r="V3" s="105" t="str">
         <f ca="1">$A$3&amp;" 08.2"</f>
-        <v>Pareja  08.2</v>
+        <v>Pair  08.2</v>
       </c>
       <c r="W3" s="132" t="str">
         <f ca="1">$A$3&amp;" 09.1"</f>
-        <v>Pareja  09.1</v>
+        <v>Pair  09.1</v>
       </c>
       <c r="X3" s="132" t="str">
         <f ca="1">$A$3&amp;" 09.2"</f>
-        <v>Pareja  09.2</v>
+        <v>Pair  09.2</v>
       </c>
       <c r="Y3" s="107" t="str">
         <f ca="1">$A$3&amp;" 10.1"</f>
-        <v>Pareja  10.1</v>
+        <v>Pair  10.1</v>
       </c>
       <c r="Z3" s="107" t="str">
         <f ca="1">$A$3&amp;" 10.2"</f>
-        <v>Pareja  10.2</v>
+        <v>Pair  10.2</v>
       </c>
       <c r="AA3" s="109" t="str">
         <f ca="1">$A$3&amp;" 11.1"</f>
-        <v>Pareja  11.1</v>
+        <v>Pair  11.1</v>
       </c>
       <c r="AB3" s="109" t="str">
         <f ca="1">$A$3&amp;" 11.2"</f>
-        <v>Pareja  11.2</v>
+        <v>Pair  11.2</v>
       </c>
       <c r="AC3" s="111" t="str">
         <f ca="1">$A$3&amp;" 12.1"</f>
-        <v>Pareja  12.1</v>
+        <v>Pair  12.1</v>
       </c>
       <c r="AD3" s="111" t="str">
         <f ca="1">$A$3&amp;" 12.1"</f>
-        <v>Pareja  12.1</v>
+        <v>Pair  12.1</v>
       </c>
       <c r="AE3" s="113" t="str">
         <f ca="1">'Datos OM'!AE3</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="114" t="str">
         <f ca="1">'Datos OM'!AF3</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="115" t="str">
         <f ca="1">'Datos OM'!AG3</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="116" t="str">
         <f ca="1">'Datos OM'!AH3</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="str">
         <f>'Datos OM'!AI3</f>
@@ -29813,7 +29825,7 @@
       <c r="AI7" s="86"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9e8Dn6Ln+pP2PHneEB5z1LQVPjNSmU8BgJiXUDytfO7ewSWILCL6gkQDZagFQMaRQ3Tt/AayZz3qaP0BoNO+gA==" saltValue="Td/S6XBYnhXbbgfta8uglA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Mmczwuw7UfSjHC4HKz855PtdJuSqtPDMCjEEB4xNcwu2oEM0WpyEdlMrMizSzzz+dvWLsstMLQkX9UVevclZtg==" saltValue="nhCLZBMI+3MAqFnyHRwzVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -29834,7 +29846,7 @@
       <selection pane="bottomRight" activeCell="D5" sqref="D5:AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="3.64453125" style="2" customWidth="1"/>
     <col min="2" max="2" width="3.64453125" style="2" hidden="1" customWidth="1"/>
@@ -29862,11 +29874,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -29899,7 +29911,7 @@
       <c r="E2"/>
       <c r="F2" s="59" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabl_RC[Enunciado])</f>
@@ -29909,135 +29921,135 @@
     <row r="3" spans="1:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="61" t="str">
         <f ca="1">INDIRECT("Z_BP_19_"&amp;IDIOMA)</f>
-        <v>Respuesta</v>
+        <v>Answer</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="18"/>
       <c r="D3" s="53" t="str">
         <f ca="1">INDIRECT("Z_BP_18_"&amp;IDIOMA)</f>
-        <v>Mayúsculas</v>
+        <v>Capitalization</v>
       </c>
       <c r="E3" s="22" t="str">
         <f ca="1">'Datos OM'!E3</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!K24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - RESPUESTA CORTA
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - SHORT ANSWER
+Question statement</v>
       </c>
       <c r="G3" s="103" t="str">
         <f ca="1">$A$3&amp;" 01"</f>
-        <v>Respuesta 01</v>
+        <v>Answer 01</v>
       </c>
       <c r="H3" s="104" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 01"</f>
-        <v>Puntos 01</v>
+        <v>Points 01</v>
       </c>
       <c r="I3" s="104" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 01"</f>
-        <v>Retroalim. 01</v>
+        <v>Feedback 01</v>
       </c>
       <c r="J3" s="105" t="str">
         <f ca="1">$A$3&amp;" 02"</f>
-        <v>Respuesta 02</v>
+        <v>Answer 02</v>
       </c>
       <c r="K3" s="106" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 02"</f>
-        <v>Puntos 02</v>
+        <v>Points 02</v>
       </c>
       <c r="L3" s="106" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 02"</f>
-        <v>Retroalim. 02</v>
+        <v>Feedback 02</v>
       </c>
       <c r="M3" s="105" t="str">
         <f ca="1">$A$3&amp;" 03"</f>
-        <v>Respuesta 03</v>
+        <v>Answer 03</v>
       </c>
       <c r="N3" s="106" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 03"</f>
-        <v>Puntos 03</v>
+        <v>Points 03</v>
       </c>
       <c r="O3" s="106" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 03"</f>
-        <v>Retroalim. 03</v>
+        <v>Feedback 03</v>
       </c>
       <c r="P3" s="107" t="str">
         <f ca="1">$A$3&amp;" 04"</f>
-        <v>Respuesta 04</v>
+        <v>Answer 04</v>
       </c>
       <c r="Q3" s="108" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 04"</f>
-        <v>Puntos 04</v>
+        <v>Points 04</v>
       </c>
       <c r="R3" s="108" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 04"</f>
-        <v>Retroalim. 04</v>
+        <v>Feedback 04</v>
       </c>
       <c r="S3" s="109" t="str">
         <f ca="1">$A$3&amp;" 05"</f>
-        <v>Respuesta 05</v>
+        <v>Answer 05</v>
       </c>
       <c r="T3" s="110" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 05"</f>
-        <v>Puntos 05</v>
+        <v>Points 05</v>
       </c>
       <c r="U3" s="110" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 05"</f>
-        <v>Retroalim. 05</v>
+        <v>Feedback 05</v>
       </c>
       <c r="V3" s="111" t="str">
         <f ca="1">$A$3&amp;" 06"</f>
-        <v>Respuesta 06</v>
+        <v>Answer 06</v>
       </c>
       <c r="W3" s="112" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 06"</f>
-        <v>Puntos 06</v>
+        <v>Points 06</v>
       </c>
       <c r="X3" s="112" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 06"</f>
-        <v>Retroalim. 06</v>
+        <v>Feedback 06</v>
       </c>
       <c r="Y3" s="103" t="str">
         <f ca="1">$A$3&amp;" 07"</f>
-        <v>Respuesta 07</v>
+        <v>Answer 07</v>
       </c>
       <c r="Z3" s="104" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 07"</f>
-        <v>Puntos 07</v>
+        <v>Points 07</v>
       </c>
       <c r="AA3" s="104" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 07"</f>
-        <v>Retroalim. 07</v>
+        <v>Feedback 07</v>
       </c>
       <c r="AB3" s="105" t="str">
         <f ca="1">$A$3&amp;" 08"</f>
-        <v>Respuesta 08</v>
+        <v>Answer 08</v>
       </c>
       <c r="AC3" s="106" t="str">
         <f ca="1">INDIRECT("Z_BP_09_"&amp;IDIOMA)&amp;" 08"</f>
-        <v>Puntos 08</v>
+        <v>Points 08</v>
       </c>
       <c r="AD3" s="106" t="str">
         <f ca="1">INDIRECT("Z_BP_07_"&amp;IDIOMA)&amp;" 08"</f>
-        <v>Retroalim. 08</v>
+        <v>Feedback 08</v>
       </c>
       <c r="AE3" s="113" t="str">
         <f ca="1">'Datos OM'!AE3</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="114" t="str">
         <f ca="1">'Datos OM'!AF3</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="115" t="str">
         <f ca="1">'Datos OM'!AG3</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="116" t="str">
         <f ca="1">'Datos OM'!AH3</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="str">
         <f>'Datos OM'!AI3</f>
@@ -30312,7 +30324,7 @@
       <c r="AI6" s="86"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AS9vNWAtTWa4xiG5Ydft4nR4f+lcu2mQqfZAPq3YdHsVAi2IWm+zCXMPILpOAAFs2ZTdSFWQjW8eMlfY56k8Nw==" saltValue="KJkj8WkoK7/8LF7gOFaaVw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="GjG5KGJEaM+kVJa1x387Lrk99gOkQD78eEw52mAJfWI9/YgJbl8LfS73u/8zjfrz95ryUdbi3oQ+slQvtSuVtw==" saltValue="t6Uufg2zZTbXGW8JbB0zUA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -30330,10 +30342,10 @@
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5:AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -30355,11 +30367,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -30392,7 +30404,7 @@
       <c r="E2"/>
       <c r="F2" s="59" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_PP[Enunciado])</f>
@@ -30402,156 +30414,156 @@
     <row r="3" spans="1:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="64" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)</f>
-        <v xml:space="preserve">Palabra </v>
+        <v xml:space="preserve">Word </v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="11" t="str">
         <f ca="1">'Datos OM'!E3</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!M24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - PALABRA PERDIDA
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - MISSING WORD
+Question statement</v>
       </c>
       <c r="G3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;H3</f>
-        <v>Grupo 
-Palabra  01</v>
+        <v>Group 
+Word  01</v>
       </c>
       <c r="H3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 01"</f>
-        <v>Palabra  01</v>
+        <v>Word  01</v>
       </c>
       <c r="I3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;J3</f>
-        <v>Grupo 
-Palabra  02</v>
+        <v>Group 
+Word  02</v>
       </c>
       <c r="J3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 02"</f>
-        <v>Palabra  02</v>
+        <v>Word  02</v>
       </c>
       <c r="K3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;L3</f>
-        <v>Grupo 
-Palabra  03</v>
+        <v>Group 
+Word  03</v>
       </c>
       <c r="L3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 03"</f>
-        <v>Palabra  03</v>
+        <v>Word  03</v>
       </c>
       <c r="M3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;N3</f>
-        <v>Grupo 
-Palabra  04</v>
+        <v>Group 
+Word  04</v>
       </c>
       <c r="N3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 04"</f>
-        <v>Palabra  04</v>
+        <v>Word  04</v>
       </c>
       <c r="O3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;P3</f>
-        <v>Grupo 
-Palabra  05</v>
+        <v>Group 
+Word  05</v>
       </c>
       <c r="P3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 05"</f>
-        <v>Palabra  05</v>
+        <v>Word  05</v>
       </c>
       <c r="Q3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;R3</f>
-        <v>Grupo 
-Palabra  06</v>
+        <v>Group 
+Word  06</v>
       </c>
       <c r="R3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 06"</f>
-        <v>Palabra  06</v>
+        <v>Word  06</v>
       </c>
       <c r="S3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;T3</f>
-        <v>Grupo 
-Palabra  07</v>
+        <v>Group 
+Word  07</v>
       </c>
       <c r="T3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 07"</f>
-        <v>Palabra  07</v>
+        <v>Word  07</v>
       </c>
       <c r="U3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;V3</f>
-        <v>Grupo 
-Palabra  08</v>
+        <v>Group 
+Word  08</v>
       </c>
       <c r="V3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 08"</f>
-        <v>Palabra  08</v>
+        <v>Word  08</v>
       </c>
       <c r="W3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;X3</f>
-        <v>Grupo 
-Palabra  09</v>
+        <v>Group 
+Word  09</v>
       </c>
       <c r="X3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 09"</f>
-        <v>Palabra  09</v>
+        <v>Word  09</v>
       </c>
       <c r="Y3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;Z3</f>
-        <v>Grupo 
-Palabra  10</v>
+        <v>Group 
+Word  10</v>
       </c>
       <c r="Z3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 10"</f>
-        <v>Palabra  10</v>
+        <v>Word  10</v>
       </c>
       <c r="AA3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;AB3</f>
-        <v>Grupo 
-Palabra  11</v>
+        <v>Group 
+Word  11</v>
       </c>
       <c r="AB3" s="117" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 11"</f>
-        <v>Palabra  11</v>
+        <v>Word  11</v>
       </c>
       <c r="AC3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_23_"&amp;IDIOMA)&amp;"
 "&amp;AD3</f>
-        <v>Grupo 
-Palabra  12</v>
+        <v>Group 
+Word  12</v>
       </c>
       <c r="AD3" s="118" t="str">
         <f ca="1">INDIRECT("Z_BP_20_"&amp;IDIOMA)&amp;" 12"</f>
-        <v>Palabra  12</v>
+        <v>Word  12</v>
       </c>
       <c r="AE3" s="113" t="str">
         <f ca="1">'Datos OM'!AE3</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="114" t="str">
         <f ca="1">'Datos OM'!AF3</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="115" t="str">
         <f ca="1">'Datos OM'!AG3</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="116" t="str">
         <f ca="1">'Datos OM'!AH3</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="str">
         <f>'Datos OM'!AI3</f>
@@ -30866,7 +30878,7 @@
       <c r="AI6" s="86"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q9s/6o2jIDuV+iYV/xjM4Cuff/s4UDKJNzjYMGMZz52zHKuky1hsXynPzGh5wuLus1olYqnP63rSABj/5fwTUA==" saltValue="cybCVNG9puXGIH+c0MuEGw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -30887,7 +30899,7 @@
       <selection pane="bottomRight" activeCell="E5" sqref="E5:AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -30914,11 +30926,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -30951,7 +30963,7 @@
       <c r="E2"/>
       <c r="F2" s="59" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_EN[FastTest PlugIn - ENSAYO
@@ -30966,43 +30978,43 @@
       <c r="D3" s="18"/>
       <c r="E3" s="11" t="str">
         <f ca="1">'Datos OM'!E3</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!O24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
-        <v>FastTest PlugIn - V7.8  - ENSAYO
-Enunciado de la pregunta</v>
+        <v>FastTest PlugIn - V7.8  - ESSAY
+Question statement</v>
       </c>
       <c r="G3" s="55" t="str">
         <f ca="1">INDIRECT("Z_BP_24_"&amp;IDIOMA)&amp;"
 "&amp;H3</f>
-        <v>Formato de la Respuesta
-Requerir texto</v>
+        <v>Response format
+Require text</v>
       </c>
       <c r="H3" s="74" t="str">
         <f ca="1">INDIRECT("Z_BP_25_"&amp;IDIOMA)</f>
-        <v>Requerir texto</v>
+        <v>Require text</v>
       </c>
       <c r="I3" s="69" t="str">
         <f ca="1">INDIRECT("Z_BP_26_"&amp;IDIOMA)</f>
-        <v>Tamaño de la caja de entrada</v>
+        <v>Input box size</v>
       </c>
       <c r="J3" s="56" t="str">
         <f ca="1">INDIRECT("Z_BP_27_"&amp;IDIOMA)</f>
-        <v>Permitir archivos adjuntos</v>
+        <v>Allow attachments</v>
       </c>
       <c r="K3" s="57" t="str">
         <f ca="1">INDIRECT("Z_BP_28_"&amp;IDIOMA)</f>
-        <v>Archivos adjuntos requeridos</v>
+        <v>Require attachments</v>
       </c>
       <c r="L3" s="58" t="str">
         <f ca="1">INDIRECT("Z_BP_29_"&amp;IDIOMA)</f>
-        <v>Plantilla de Respuesta</v>
+        <v>Response template</v>
       </c>
       <c r="M3" s="55" t="str">
         <f ca="1">INDIRECT("Z_BP_30_"&amp;IDIOMA)</f>
-        <v>Información para el evaluador</v>
+        <v>Information for graders</v>
       </c>
       <c r="N3" s="122"/>
       <c r="O3" s="123"/>
@@ -31246,12 +31258,12 @@
       <c r="AI6" s="86"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="EmdZmzT6nbbsdWiQI3OR8ck6Uujyp5cw3+iZM3WynJgRLqQYUfzTJ/pZSDClwvZKKZM+g8je4oiatl6UMfuXvQ==" saltValue="311fgeu1MWcEHoyhQJLA1g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="JxgCs+G3EEwK9EqpfVj2svZMtqjKaxeZPfCNjoaNlb6fWerjgQnsPwKnMVh6cnJy0ZsfQd1LLG7rW416ROaqig==" saltValue="BArQLDR5OfpVdFqW7RpFKg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <conditionalFormatting sqref="G5:K6">
-    <cfRule type="cellIs" dxfId="119" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31266,16 +31278,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Hoja_28"/>
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5:AI5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5:AI7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="3.64453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="3.52734375" hidden="1" customWidth="1"/>
@@ -31298,11 +31310,11 @@
       <c r="E1" s="35"/>
       <c r="F1" s="59" t="str">
         <f ca="1">'Datos OM'!F1</f>
-        <v>OM 1R                  OM +R                    VF                         EM                                INICIO</v>
+        <v>MC 1A                  MC +A                    TF                         MA                                HOME</v>
       </c>
       <c r="G1" s="51" t="str">
         <f ca="1">INDIRECT("Z_BP_01_"&amp;IDIOMA)</f>
-        <v>Preguntas Almacenadas</v>
+        <v>Saved Questions</v>
       </c>
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
@@ -31334,11 +31346,11 @@
       <c r="E2"/>
       <c r="F2" s="60" t="str">
         <f ca="1">'Datos OM'!F2</f>
-        <v xml:space="preserve">    RC                         PP                         EN                         CL                                 DICCIONARIO</v>
+        <v xml:space="preserve">    SA                         MW                         ES                         CL                                 DICTIONARY</v>
       </c>
       <c r="G2" s="34">
         <f>COUNTA(Tabla_CL[Enunciado])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
@@ -31348,22 +31360,22 @@
       <c r="D3" s="18"/>
       <c r="E3" s="22" t="str">
         <f ca="1">'Datos OM'!E3</f>
-        <v>Descripción</v>
+        <v>Description</v>
       </c>
       <c r="F3" s="36" t="str">
         <f ca="1">"FastTest PlugIn - V"&amp;MID(Version,5,7)&amp;UPPER(INICIO!Q24)&amp;"
 "&amp;INDIRECT("Z_BP_03_"&amp;IDIOMA)</f>
         <v>FastTest PlugIn - V7.8  - CLOZE
-Enunciado de la pregunta</v>
+Question statement</v>
       </c>
       <c r="G3" s="133" t="str">
         <f ca="1">INDIRECT("Z_BP_32_"&amp;IDIOMA)</f>
-        <v>Ancho RC</v>
+        <v>Width SA</v>
       </c>
       <c r="H3" s="74"/>
       <c r="I3" s="69" t="str">
         <f ca="1">MID(G3,1,SEARCH(" ",G3,1))&amp;AI3</f>
-        <v>Ancho Imagen</v>
+        <v>Width Imagen</v>
       </c>
       <c r="J3" s="56"/>
       <c r="K3" s="57"/>
@@ -31388,19 +31400,19 @@
       <c r="AD3" s="121"/>
       <c r="AE3" s="113" t="str">
         <f ca="1">'Datos OM'!AE3</f>
-        <v>Pista 1</v>
+        <v>Hint 1</v>
       </c>
       <c r="AF3" s="114" t="str">
         <f ca="1">'Datos OM'!AF3</f>
-        <v>Pista 2</v>
+        <v>Hint 2</v>
       </c>
       <c r="AG3" s="115" t="str">
         <f ca="1">'Datos OM'!AG3</f>
-        <v>Pista 3</v>
+        <v>Hint 3</v>
       </c>
       <c r="AH3" s="116" t="str">
         <f ca="1">'Datos OM'!AH3</f>
-        <v>Pista 4</v>
+        <v>Hint 4</v>
       </c>
       <c r="AI3" s="65" t="str">
         <f>'Datos OM'!AI3</f>
@@ -31526,9 +31538,11 @@
         <v>971</v>
       </c>
       <c r="G5" s="163">
-        <v>10</v>
-      </c>
-      <c r="H5" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="H5" s="25">
+        <v>50</v>
+      </c>
       <c r="I5" s="14"/>
       <c r="J5" s="129"/>
       <c r="K5" s="130"/>
@@ -31557,8 +31571,106 @@
       <c r="AH5" s="167"/>
       <c r="AI5" s="86"/>
     </row>
+    <row r="6" spans="1:35" ht="81.7" x14ac:dyDescent="0.5">
+      <c r="A6" s="175"/>
+      <c r="B6" s="176"/>
+      <c r="C6" s="152"/>
+      <c r="D6" s="152"/>
+      <c r="E6" s="77" t="s">
+        <v>972</v>
+      </c>
+      <c r="F6" s="151" t="s">
+        <v>973</v>
+      </c>
+      <c r="G6" s="163">
+        <v>15</v>
+      </c>
+      <c r="H6" s="25">
+        <v>200</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="157"/>
+      <c r="O6" s="158"/>
+      <c r="P6" s="158"/>
+      <c r="Q6" s="157"/>
+      <c r="R6" s="157"/>
+      <c r="S6" s="158"/>
+      <c r="T6" s="158"/>
+      <c r="U6" s="157"/>
+      <c r="V6" s="157"/>
+      <c r="W6" s="158"/>
+      <c r="X6" s="158"/>
+      <c r="Y6" s="157"/>
+      <c r="Z6" s="157"/>
+      <c r="AA6" s="158"/>
+      <c r="AB6" s="158"/>
+      <c r="AC6" s="157"/>
+      <c r="AD6" s="157"/>
+      <c r="AE6" s="164" t="s">
+        <v>921</v>
+      </c>
+      <c r="AF6" s="165" t="s">
+        <v>921</v>
+      </c>
+      <c r="AG6" s="166" t="s">
+        <v>921</v>
+      </c>
+      <c r="AH6" s="167" t="s">
+        <v>921</v>
+      </c>
+      <c r="AI6" s="86" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="23.35" x14ac:dyDescent="0.5">
+      <c r="A7" s="175"/>
+      <c r="B7" s="176"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="77" t="s">
+        <v>974</v>
+      </c>
+      <c r="F7" s="151" t="s">
+        <v>975</v>
+      </c>
+      <c r="G7" s="163">
+        <v>15</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="128"/>
+      <c r="N7" s="157"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="158"/>
+      <c r="Q7" s="157"/>
+      <c r="R7" s="157"/>
+      <c r="S7" s="158"/>
+      <c r="T7" s="158"/>
+      <c r="U7" s="157"/>
+      <c r="V7" s="157"/>
+      <c r="W7" s="158"/>
+      <c r="X7" s="158"/>
+      <c r="Y7" s="157"/>
+      <c r="Z7" s="157"/>
+      <c r="AA7" s="158"/>
+      <c r="AB7" s="158"/>
+      <c r="AC7" s="157"/>
+      <c r="AD7" s="157"/>
+      <c r="AE7" s="164"/>
+      <c r="AF7" s="165"/>
+      <c r="AG7" s="166"/>
+      <c r="AH7" s="167"/>
+      <c r="AI7" s="86"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="20ikIbEfLDSZ70Kzq/bIOpMey9FS9D60F7YyPMOwht/ewhZ8+LTbH3kooqqa39uOCrUKDvMvhrFVO0XnXHYIVQ==" saltValue="pX+vmvycEnzuDWtVdBWf/g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="agMVMEDegok9+6tCOZxqE049Dy64pua8BaNuTpL6oqpVBX3W9OvJwyuIVpxNrbWvtKFj1mJ4TLZdcpizPDNLnw==" saltValue="gTRA/ii0q9sQ1PB4ghaYeA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="1">
     <mergeCell ref="A3:B3"/>
   </mergeCells>

</xml_diff>